<commit_message>
Seperated the admin from the app.js and also updated the README and quests.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Quests/quests.xlsx
+++ b/resources/data-imports/Quests/quests.xlsx
@@ -2618,7 +2618,7 @@
         <v>28</v>
       </c>
       <c r="H19">
-        <v>25000</v>
+        <v>5000</v>
       </c>
       <c r="L19" t="s">
         <v>120</v>
@@ -2644,7 +2644,7 @@
         <v>28</v>
       </c>
       <c r="H20">
-        <v>25000</v>
+        <v>5000</v>
       </c>
       <c r="L20" t="s">
         <v>124</v>
@@ -2673,7 +2673,7 @@
         <v>124</v>
       </c>
       <c r="H21">
-        <v>30000</v>
+        <v>8000</v>
       </c>
       <c r="L21" t="s">
         <v>128</v>
@@ -2702,7 +2702,7 @@
         <v>128</v>
       </c>
       <c r="H22">
-        <v>50000</v>
+        <v>12000</v>
       </c>
       <c r="L22" t="s">
         <v>132</v>
@@ -2731,7 +2731,7 @@
         <v>132</v>
       </c>
       <c r="H23">
-        <v>75000</v>
+        <v>15000</v>
       </c>
       <c r="L23" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
Lots of changes and fixes and event more tests added and some refactorings.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Quests/quests.xlsx
+++ b/resources/data-imports/Quests/quests.xlsx
@@ -1601,85 +1601,85 @@
     <t>The Child's Journal</t>
   </si>
   <si>
+    <t>Bloody Snowball</t>
+  </si>
+  <si>
+    <t>You stare at The Soldiers Brother for a moment and then ask him what any of this has to do with anything?&lt;br /&gt; &lt;br /&gt; “The night we came to find The Child, he was long gone. The night we we came to find The Child was the night they found the truth. That was the night my Father banished my brother to the cold and told him to never look back for The Church would be hunting him for his crimes against God.”&lt;br /&gt; &lt;br /&gt; That’s when it hit you.&lt;br /&gt; &lt;br /&gt; The Soldier’s forbidden love … Was his brother.</t>
+  </si>
+  <si>
+    <t>You hold in your hand a Bloody Shirt that you found on a wondering creature. You stepped outside after the story, two brothers. Two lovers. Was it unholy, was it unnatural? Maybe. With everything you have seen, the death, the pain, the infliction of confusion and the haunting torment that follows you across the various planes comes the question of who is one to judge who one loves in these times.&lt;br /&gt; &lt;br /&gt; So what did this story have to do with The Child? You remember the journal and flip through its pages only to find an entry:&lt;br /&gt; &lt;br /&gt; “The Child found a wondering man, a drunkard who was aimless and seeking a direction in life. One who seemed like had everything stolen from him. It was the night the snow fell and The Child celebrated the coming new year with those he considered his friends: The Red Hawk Soldiers. Neither The Child nor his companions knew who this drunkard really was, they welcomed him among their ranks.”&lt;br /&gt; &lt;br /&gt; The Soldier joined The Child in his fight against The Church and The Federation, The Federation was where his father was. It made sense now as to how the two are indirectly tied.&lt;br /&gt; &lt;br /&gt; “There's something I need, something that can help you in your war against The Ice Queen and her frozen lands.”&lt;br /&gt; &lt;br /&gt; You turn and see The Soldiers Brother standing before you.&lt;br /&gt; &lt;br /&gt; “Do this for me, and ill give you something that will let you control the land around you.”</t>
+  </si>
+  <si>
+    <t>The Experiments</t>
+  </si>
+  <si>
+    <t>Trix</t>
+  </si>
+  <si>
+    <t>Pages of the holy book</t>
+  </si>
+  <si>
+    <t>You ask the child what he means by: The whisper of the past is coming back like a scream.&lt;br /&gt; &lt;br /&gt; “I understand not what you ask child. But I do have something to share with you. The Church holds a secret unlike any other. It is said that The Church has started to practice the art of Alchemy. They had texts and magical research in their studies and in the research areas. They even practiced their twisted magics on the children – to make them more holy.”&lt;br /&gt; &lt;br /&gt; You might be able to find some of the pages around here, they called it their holy book.</t>
+  </si>
+  <si>
+    <t>You managed to find some torn pages around the area that detail the horrific experiments and abuses done to the children by those at The Church who practiced a different kind of alchemy, a darker more twisted version of it’s self.&lt;br /&gt; &lt;br /&gt; They detail the experiments and the outcomes of turning these children in to more holy elevated beings, only for the experiments to have failed and instead corrupt their souls causing the priests and the soldiers to have to put the children down.&lt;br /&gt; &lt;br /&gt; You hand the pages over to Trix and ask what use they are to him.&lt;br /&gt; &lt;br /&gt; “They are of no use to me child, they are for you to understand why it happened.”&lt;br /&gt; &lt;br /&gt; Why what happened the experiments?&lt;br /&gt; &lt;br /&gt; “No. The raid.”</t>
+  </si>
+  <si>
+    <t>The Memories and The War Plans</t>
+  </si>
+  <si>
+    <t>Box of Memories</t>
+  </si>
+  <si>
+    <t>Child's Drawings</t>
+  </si>
+  <si>
+    <t>“The night the snow stopped falling was the night they moved in silence through these fields, it was also the night they invaded The Church.” Trix began.&lt;br /&gt; &lt;br /&gt; “They came in the silence and they slaughtered the priests in their studies. They discovered the travesties that were taking place and put those responsible down. They saved us. I remember him, The Creator – although then he was known as The Child. He saved me. He gave me a box I lost around here. I gave him the drawings – he might have lost them as well, but they were like a map. A map through the church.</t>
+  </si>
+  <si>
+    <t>You found the box and the drawings and handed them over to Trix.&lt;br /&gt; &lt;br /&gt; “That was the last night I knew pain and suffering. Or so I thought.” Trix began.&lt;br /&gt; &lt;br /&gt; “They, the Red Hawk Soldiers and The Child took us, the remaining children to hide out at what is now known as The Abandoned Village. A few months later it burned to the ground. A few months later it was attacked by The Federation. They came, they burned, raped, pillaged, destroyed, slaughtered everything in their path – in the name of retribution.”&lt;br /&gt; &lt;br /&gt; he pauses to stare at his toy box and the drawings. The snow starts to fall again and the silence is as deafening as it ever was.&lt;br /&gt; &lt;br /&gt; “The Child escaped.” He continued.&lt;br /&gt; &lt;br /&gt; “The Child escaped.”</t>
+  </si>
+  <si>
+    <t>The Sword and The Door</t>
+  </si>
+  <si>
+    <t>Red Hawks Sword</t>
+  </si>
+  <si>
+    <t>The Letter</t>
+  </si>
+  <si>
+    <t>You search the area for Trix but he is no where to be found. The snow falls more heavily now and you start to think back on your time here in this world. It’s dark, twisted, broken and frozen landscapes contrast with that of the inhabitants, lost memories and ghosts of another time ruled by a mad queen who can’t let go of the grief and loss she has suffered.&lt;br /&gt; &lt;br /&gt; It all starts to make sense now, it’s all connected to The Creator, its all connected to his story, to his own inability to let go, to crave peace and happiness as opposed to living in the darkness and depravity of his own twisted disillusion and self inflicted madness.&lt;br /&gt; &lt;br /&gt; But why not let go? What do you cling to? What memory, what hope – what fleeting light do you grasp to. Why keep all this alive? What does it serve you in the end?</t>
+  </si>
+  <si>
+    <t>You stumble across a sword in the snow guarded by fearsome creatures you slaughter. You spill their blood upon the snow already stained with the blood of the past and its twisted memories.&lt;br /&gt; &lt;br /&gt; “You found the sword.” Comes a familiar and small voice of said past. Trix stands before you in the snow looking at the sword. You ask what the significance of the sword is and he states its nothing, its a symbol of the night the raid took place, of the night they rescued the children from the horrors of what would have been.&lt;br /&gt; &lt;br /&gt; You ask about the abandoned village stating that the story of his death didn’t make sense with that of The Queens.&lt;br /&gt; &lt;br /&gt; “Death takes place in different timelines, but in the same place at the same time – causing the paradox before you. Two places, two different timelines, the exact same time. Its how she got here. My death opened the door for her to come, she just chose to never leave.”&lt;br /&gt; &lt;br /&gt; This makes you wonder – did The Creator come through a door?&lt;br /&gt; &lt;br /&gt; “Here.” Trix hands you an envelope. You ask what it is.&lt;br /&gt; &lt;br /&gt; “A letter to the Soldier from his brother. Take it to him. He has something for you.”&lt;br /&gt; &lt;br /&gt; What could he have?</t>
+  </si>
+  <si>
+    <t>Reuniting Two Old Flames</t>
+  </si>
+  <si>
+    <t>Ice Queens Treaty Scrolls</t>
+  </si>
+  <si>
+    <t>You arrive at a pub in Smugglers Port where you see The Soldier sitting alone at a table drinking.&lt;br /&gt; &lt;br /&gt; You sit down across from him and he greets you with a warm smile. “What brings you here child?”&lt;br /&gt; &lt;br /&gt; You explain the adventures you have been on, the Ice Plane, The Queen, The Creator, How it is all connected together. You then explain the story about his brother and he stops you.&lt;br /&gt; &lt;br /&gt; “That is something we do not talk about child. My past is mine alone and I wont have you meddling it in with your stories of nonsense.”&lt;br /&gt; &lt;br /&gt; The Soldier stands and snatches the letter from your hands.&lt;br /&gt; &lt;br /&gt; “You dare not to travel down this road child. You will regret it.”</t>
+  </si>
+  <si>
+    <t>You stand alone on the docks of Smugglers Port waiting for The Soldier to arrive. You see him walking down the docks to meet you.&lt;br /&gt; &lt;br /&gt; “What is it you want child?”&lt;br /&gt; &lt;br /&gt; You grab his hand and utter the words, and before he can protest you and The Soldier stand in the middle of a frozen road. He turns and sees the familiar sign, the words – its haunts him – written all over his face: Gas and Sip.&lt;br /&gt; &lt;br /&gt; “How could you!” He screams.&lt;br /&gt; &lt;br /&gt; “Brother.” Comes a familiar voice.&lt;br /&gt; &lt;br /&gt; The two brothers stand face to face in the frozen desolate landscape of memories better left to rot in the darkness of their own twisted depravity. But there is something beautiful in the reuniting of two brothers, two lovers. Two sinners.&lt;br /&gt; &lt;br /&gt; “I have something for you.” The Soldiers Brother begins. “For doing me this favor.”&lt;br /&gt; &lt;br /&gt; He hands you a scroll.&lt;br /&gt; &lt;br /&gt; “With this, you can settle any where you please. You will find these lands to be much more hostile then where you come from child.”</t>
+  </si>
+  <si>
+    <t>Broken Road</t>
+  </si>
+  <si>
+    <t>It has been weeks since you last entered the house to face the shadows of the The Creator and his own families memories of pain and misery.&lt;br /&gt; &lt;br /&gt; You have walked into the wilderness looking for more answers to the past, looking for a way to kill The Ice Queen.&lt;br /&gt; &lt;br /&gt; You have been told by The Poet that their might be story of answers to the west, along the old broken road that leads to the abandoned church.&lt;br /&gt; &lt;br /&gt; You ask him what could possibly be over there that could be of help in this frozen waste land.&lt;br /&gt; &lt;br /&gt; “The ability to declare war upon her land child.” He smiles as he states this.&lt;br /&gt; &lt;br /&gt; “Seek out the soldiers brother, his own father was a great general.”</t>
+  </si>
+  <si>
+    <t>You arrive at the road, snow covered with trees off to the side, the road travels through a dark forest, whose trees are covered in lights. Lights that glow red, green and blue. There is sparkly hanging tinsel through out the trees.&lt;br /&gt; &lt;br /&gt; You slowly begin the travel don the road and feel the wind get colder, the snow falls more heavily here and seek out some kind of shelter.&lt;br /&gt; &lt;br /&gt; Off to the distance you see an old building, as you get closer you can read a fading title: Gas and Sip, what ever that means.&lt;br /&gt; &lt;br /&gt; You enter the abandoned building and see a counter as well as isles of empty shelves.&lt;br /&gt; &lt;br /&gt; You turn around and a handsome blonde, blue eyed man no older then 28 stands before you. Clad in leather Armour and carrying a short sword he stairs you down.</t>
+  </si>
+  <si>
+    <t>The Soldiers Forbidden Love</t>
+  </si>
+  <si>
     <t>The Soldiers Journal</t>
-  </si>
-  <si>
-    <t>Bloody Snowball</t>
-  </si>
-  <si>
-    <t>You stare at The Soldiers Brother for a moment and then ask him what any of this has to do with anything?&lt;br /&gt; &lt;br /&gt; “The night we came to find The Child, he was long gone. The night we we came to find The Child was the night they found the truth. That was the night my Father banished my brother to the cold and told him to never look back for The Church would be hunting him for his crimes against God.”&lt;br /&gt; &lt;br /&gt; That’s when it hit you.&lt;br /&gt; &lt;br /&gt; The Soldier’s forbidden love … Was his brother.</t>
-  </si>
-  <si>
-    <t>You hold in your hand a Bloody Shirt that you found on a wondering creature. You stepped outside after the story, two brothers. Two lovers. Was it unholy, was it unnatural? Maybe. With everything you have seen, the death, the pain, the infliction of confusion and the haunting torment that follows you across the various planes comes the question of who is one to judge who one loves in these times.&lt;br /&gt; &lt;br /&gt; So what did this story have to do with The Child? You remember the journal and flip through its pages only to find an entry:&lt;br /&gt; &lt;br /&gt; “The Child found a wondering man, a drunkard who was aimless and seeking a direction in life. One who seemed like had everything stolen from him. It was the night the snow fell and The Child celebrated the coming new year with those he considered his friends: The Red Hawk Soldiers. Neither The Child nor his companions knew who this drunkard really was, they welcomed him among their ranks.”&lt;br /&gt; &lt;br /&gt; The Soldier joined The Child in his fight against The Church and The Federation, The Federation was where his father was. It made sense now as to how the two are indirectly tied.&lt;br /&gt; &lt;br /&gt; “There's something I need, something that can help you in your war against The Ice Queen and her frozen lands.”&lt;br /&gt; &lt;br /&gt; You turn and see The Soldiers Brother standing before you.&lt;br /&gt; &lt;br /&gt; “Do this for me, and ill give you something that will let you control the land around you.”</t>
-  </si>
-  <si>
-    <t>The Experiments</t>
-  </si>
-  <si>
-    <t>Trix</t>
-  </si>
-  <si>
-    <t>Pages of the holy book</t>
-  </si>
-  <si>
-    <t>You ask the child what he means by: The whisper of the past is coming back like a scream.&lt;br /&gt; &lt;br /&gt; “I understand not what you ask child. But I do have something to share with you. The Church holds a secret unlike any other. It is said that The Church has started to practice the art of Alchemy. They had texts and magical research in their studies and in the research areas. They even practiced their twisted magics on the children – to make them more holy.”&lt;br /&gt; &lt;br /&gt; You might be able to find some of the pages around here, they called it their holy book.</t>
-  </si>
-  <si>
-    <t>You managed to find some torn pages around the area that detail the horrific experiments and abuses done to the children by those at The Church who practiced a different kind of alchemy, a darker more twisted version of it’s self.&lt;br /&gt; &lt;br /&gt; They detail the experiments and the outcomes of turning these children in to more holy elevated beings, only for the experiments to have failed and instead corrupt their souls causing the priests and the soldiers to have to put the children down.&lt;br /&gt; &lt;br /&gt; You hand the pages over to Trix and ask what use they are to him.&lt;br /&gt; &lt;br /&gt; “They are of no use to me child, they are for you to understand why it happened.”&lt;br /&gt; &lt;br /&gt; Why what happened the experiments?&lt;br /&gt; &lt;br /&gt; “No. The raid.”</t>
-  </si>
-  <si>
-    <t>The Memories and The War Plans</t>
-  </si>
-  <si>
-    <t>Box of Memories</t>
-  </si>
-  <si>
-    <t>Child's Drawings</t>
-  </si>
-  <si>
-    <t>“The night the snow stopped falling was the night they moved in silence through these fields, it was also the night they invaded The Church.” Trix began.&lt;br /&gt; &lt;br /&gt; “They came in the silence and they slaughtered the priests in their studies. They discovered the travesties that were taking place and put those responsible down. They saved us. I remember him, The Creator – although then he was known as The Child. He saved me. He gave me a box I lost around here. I gave him the drawings – he might have lost them as well, but they were like a map. A map through the church.</t>
-  </si>
-  <si>
-    <t>You found the box and the drawings and handed them over to Trix.&lt;br /&gt; &lt;br /&gt; “That was the last night I knew pain and suffering. Or so I thought.” Trix began.&lt;br /&gt; &lt;br /&gt; “They, the Red Hawk Soldiers and The Child took us, the remaining children to hide out at what is now known as The Abandoned Village. A few months later it burned to the ground. A few months later it was attacked by The Federation. They came, they burned, raped, pillaged, destroyed, slaughtered everything in their path – in the name of retribution.”&lt;br /&gt; &lt;br /&gt; he pauses to stare at his toy box and the drawings. The snow starts to fall again and the silence is as deafening as it ever was.&lt;br /&gt; &lt;br /&gt; “The Child escaped.” He continued.&lt;br /&gt; &lt;br /&gt; “The Child escaped.”</t>
-  </si>
-  <si>
-    <t>The Sword and The Door</t>
-  </si>
-  <si>
-    <t>Red Hawks Sword</t>
-  </si>
-  <si>
-    <t>The Letter</t>
-  </si>
-  <si>
-    <t>You search the area for Trix but he is no where to be found. The snow falls more heavily now and you start to think back on your time here in this world. It’s dark, twisted, broken and frozen landscapes contrast with that of the inhabitants, lost memories and ghosts of another time ruled by a mad queen who can’t let go of the grief and loss she has suffered.&lt;br /&gt; &lt;br /&gt; It all starts to make sense now, it’s all connected to The Creator, its all connected to his story, to his own inability to let go, to crave peace and happiness as opposed to living in the darkness and depravity of his own twisted disillusion and self inflicted madness.&lt;br /&gt; &lt;br /&gt; But why not let go? What do you cling to? What memory, what hope – what fleeting light do you grasp to. Why keep all this alive? What does it serve you in the end?</t>
-  </si>
-  <si>
-    <t>You stumble across a sword in the snow guarded by fearsome creatures you slaughter. You spill their blood upon the snow already stained with the blood of the past and its twisted memories.&lt;br /&gt; &lt;br /&gt; “You found the sword.” Comes a familiar and small voice of said past. Trix stands before you in the snow looking at the sword. You ask what the significance of the sword is and he states its nothing, its a symbol of the night the raid took place, of the night they rescued the children from the horrors of what would have been.&lt;br /&gt; &lt;br /&gt; You ask about the abandoned village stating that the story of his death didn’t make sense with that of The Queens.&lt;br /&gt; &lt;br /&gt; “Death takes place in different timelines, but in the same place at the same time – causing the paradox before you. Two places, two different timelines, the exact same time. Its how she got here. My death opened the door for her to come, she just chose to never leave.”&lt;br /&gt; &lt;br /&gt; This makes you wonder – did The Creator come through a door?&lt;br /&gt; &lt;br /&gt; “Here.” Trix hands you an envelope. You ask what it is.&lt;br /&gt; &lt;br /&gt; “A letter to the Soldier from his brother. Take it to him. He has something for you.”&lt;br /&gt; &lt;br /&gt; What could he have?</t>
-  </si>
-  <si>
-    <t>Reuniting Two Old Flames</t>
-  </si>
-  <si>
-    <t>Ice Queens Treaty Scrolls</t>
-  </si>
-  <si>
-    <t>You arrive at a pub in Smugglers Port where you see The Soldier sitting alone at a table drinking.&lt;br /&gt; &lt;br /&gt; You sit down across from him and he greets you with a warm smile. “What brings you here child?”&lt;br /&gt; &lt;br /&gt; You explain the adventures you have been on, the Ice Plane, The Queen, The Creator, How it is all connected together. You then explain the story about his brother and he stops you.&lt;br /&gt; &lt;br /&gt; “That is something we do not talk about child. My past is mine alone and I wont have you meddling it in with your stories of nonsense.”&lt;br /&gt; &lt;br /&gt; The Soldier stands and snatches the letter from your hands.&lt;br /&gt; &lt;br /&gt; “You dare not to travel down this road child. You will regret it.”</t>
-  </si>
-  <si>
-    <t>You stand alone on the docks of Smugglers Port waiting for The Soldier to arrive. You see him walking down the docks to meet you.&lt;br /&gt; &lt;br /&gt; “What is it you want child?”&lt;br /&gt; &lt;br /&gt; You grab his hand and utter the words, and before he can protest you and The Soldier stand in the middle of a frozen road. He turns and sees the familiar sign, the words – its haunts him – written all over his face: Gas and Sip.&lt;br /&gt; &lt;br /&gt; “How could you!” He screams.&lt;br /&gt; &lt;br /&gt; “Brother.” Comes a familiar voice.&lt;br /&gt; &lt;br /&gt; The two brothers stand face to face in the frozen desolate landscape of memories better left to rot in the darkness of their own twisted depravity. But there is something beautiful in the reuniting of two brothers, two lovers. Two sinners.&lt;br /&gt; &lt;br /&gt; “I have something for you.” The Soldiers Brother begins. “For doing me this favor.”&lt;br /&gt; &lt;br /&gt; He hands you a scroll.&lt;br /&gt; &lt;br /&gt; “With this, you can settle any where you please. You will find these lands to be much more hostile then where you come from child.”</t>
-  </si>
-  <si>
-    <t>Broken Road</t>
-  </si>
-  <si>
-    <t>It has been weeks since you last entered the house to face the shadows of the The Creator and his own families memories of pain and misery.&lt;br /&gt; &lt;br /&gt; You have walked into the wilderness looking for more answers to the past, looking for a way to kill The Ice Queen.&lt;br /&gt; &lt;br /&gt; You have been told by The Poet that their might be story of answers to the west, along the old broken road that leads to the abandoned church.&lt;br /&gt; &lt;br /&gt; You ask him what could possibly be over there that could be of help in this frozen waste land.&lt;br /&gt; &lt;br /&gt; “The ability to declare war upon her land child.” He smiles as he states this.&lt;br /&gt; &lt;br /&gt; “Seek out the soldiers brother, his own father was a great general.”</t>
-  </si>
-  <si>
-    <t>You arrive at the road, snow covered with trees off to the side, the road travels through a dark forest, whose trees are covered in lights. Lights that glow red, green and blue. There is sparkly hanging tinsel through out the trees.&lt;br /&gt; &lt;br /&gt; You slowly begin the travel don the road and feel the wind get colder, the snow falls more heavily here and seek out some kind of shelter.&lt;br /&gt; &lt;br /&gt; Off to the distance you see an old building, as you get closer you can read a fading title: Gas and Sip, what ever that means.&lt;br /&gt; &lt;br /&gt; You enter the abandoned building and see a counter as well as isles of empty shelves.&lt;br /&gt; &lt;br /&gt; You turn around and a handsome blonde, blue eyed man no older then 28 stands before you. Clad in leather Armour and carrying a short sword he stairs you down.</t>
-  </si>
-  <si>
-    <t>The Soldiers Forbidden Love</t>
   </si>
   <si>
     <t>“Who are you?” Asks the mysterious and handsome man. He walks around you and over to the counter where he puts his sword down and turns to face you.&lt;br /&gt; &lt;br /&gt; He clearly sees you as no threat, which might be to his detriment if you decide to take him out.&lt;br /&gt; &lt;br /&gt; You explain that you were sent here to search for The Soldiers brother, that The Poet sent you.&lt;br /&gt; &lt;br /&gt; “The Poet sent you. Did he tell you that he is responsible for my death? For my brothers pain that he carries with him now?”&lt;br /&gt; &lt;br /&gt; You step back and tell him you know nothing.&lt;br /&gt; &lt;br /&gt; “Perhaps you should gain and understanding of what you have been asked to do child.”&lt;br /&gt; &lt;br /&gt; You stare at him in confusion.</t>
@@ -6700,9 +6700,6 @@
       <c r="E110" t="s">
         <v>527</v>
       </c>
-      <c r="G110" t="s">
-        <v>528</v>
-      </c>
       <c r="H110">
         <v>5000</v>
       </c>
@@ -6710,7 +6707,7 @@
         <v>2000</v>
       </c>
       <c r="L110" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="M110">
         <v>20000</v>
@@ -6728,10 +6725,10 @@
         <v>521</v>
       </c>
       <c r="Z110" t="s">
+        <v>529</v>
+      </c>
+      <c r="AA110" t="s">
         <v>530</v>
-      </c>
-      <c r="AA110" t="s">
-        <v>531</v>
       </c>
       <c r="AC110" t="s">
         <v>527</v>
@@ -6745,13 +6742,13 @@
         <v>114</v>
       </c>
       <c r="B111" t="s">
+        <v>531</v>
+      </c>
+      <c r="C111" t="s">
         <v>532</v>
       </c>
-      <c r="C111" t="s">
+      <c r="G111" t="s">
         <v>533</v>
-      </c>
-      <c r="G111" t="s">
-        <v>534</v>
       </c>
       <c r="H111">
         <v>3000</v>
@@ -6772,10 +6769,10 @@
         <v>525</v>
       </c>
       <c r="Z111" t="s">
+        <v>534</v>
+      </c>
+      <c r="AA111" t="s">
         <v>535</v>
-      </c>
-      <c r="AA111" t="s">
-        <v>536</v>
       </c>
       <c r="AD111">
         <v>4</v>
@@ -6786,13 +6783,13 @@
         <v>115</v>
       </c>
       <c r="B112" t="s">
+        <v>536</v>
+      </c>
+      <c r="C112" t="s">
+        <v>532</v>
+      </c>
+      <c r="G112" t="s">
         <v>537</v>
-      </c>
-      <c r="C112" t="s">
-        <v>533</v>
-      </c>
-      <c r="G112" t="s">
-        <v>538</v>
       </c>
       <c r="H112">
         <v>5000</v>
@@ -6810,16 +6807,16 @@
         <v>100</v>
       </c>
       <c r="T112" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="U112" t="s">
+        <v>538</v>
+      </c>
+      <c r="Z112" t="s">
         <v>539</v>
       </c>
-      <c r="Z112" t="s">
+      <c r="AA112" t="s">
         <v>540</v>
-      </c>
-      <c r="AA112" t="s">
-        <v>541</v>
       </c>
       <c r="AD112">
         <v>4</v>
@@ -6830,13 +6827,13 @@
         <v>116</v>
       </c>
       <c r="B113" t="s">
+        <v>541</v>
+      </c>
+      <c r="C113" t="s">
+        <v>532</v>
+      </c>
+      <c r="G113" t="s">
         <v>542</v>
-      </c>
-      <c r="C113" t="s">
-        <v>533</v>
-      </c>
-      <c r="G113" t="s">
-        <v>543</v>
       </c>
       <c r="H113">
         <v>10000</v>
@@ -6845,7 +6842,7 @@
         <v>5000</v>
       </c>
       <c r="L113" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="M113">
         <v>50000</v>
@@ -6857,13 +6854,13 @@
         <v>100</v>
       </c>
       <c r="T113" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="Z113" t="s">
+        <v>544</v>
+      </c>
+      <c r="AA113" t="s">
         <v>545</v>
-      </c>
-      <c r="AA113" t="s">
-        <v>546</v>
       </c>
       <c r="AD113">
         <v>4</v>
@@ -6874,13 +6871,13 @@
         <v>117</v>
       </c>
       <c r="B114" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C114" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G114" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H114">
         <v>10000</v>
@@ -6889,7 +6886,7 @@
         <v>10000</v>
       </c>
       <c r="L114" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="M114">
         <v>20000</v>
@@ -6904,10 +6901,10 @@
         <v>525</v>
       </c>
       <c r="Z114" t="s">
+        <v>548</v>
+      </c>
+      <c r="AA114" t="s">
         <v>549</v>
-      </c>
-      <c r="AA114" t="s">
-        <v>550</v>
       </c>
       <c r="AD114">
         <v>4</v>
@@ -6918,7 +6915,7 @@
         <v>109</v>
       </c>
       <c r="B115" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C115" t="s">
         <v>526</v>
@@ -6948,10 +6945,10 @@
         <v>468</v>
       </c>
       <c r="Z115" t="s">
+        <v>551</v>
+      </c>
+      <c r="AA115" t="s">
         <v>552</v>
-      </c>
-      <c r="AA115" t="s">
-        <v>553</v>
       </c>
       <c r="AC115" t="s">
         <v>521</v>
@@ -6965,13 +6962,13 @@
         <v>110</v>
       </c>
       <c r="B116" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C116" t="s">
         <v>526</v>
       </c>
       <c r="G116" t="s">
-        <v>528</v>
+        <v>554</v>
       </c>
       <c r="H116">
         <v>2000</v>
@@ -6992,7 +6989,7 @@
         <v>100</v>
       </c>
       <c r="T116" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="Z116" t="s">
         <v>555</v>
@@ -7033,7 +7030,7 @@
         <v>100</v>
       </c>
       <c r="T117" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="Z117" t="s">
         <v>558</v>
@@ -7100,7 +7097,7 @@
         <v>563</v>
       </c>
       <c r="E119" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H119">
         <v>25000</v>
@@ -7133,7 +7130,7 @@
         <v>563</v>
       </c>
       <c r="AC119" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AD119">
         <v>4</v>

</xml_diff>

<commit_message>
Added a reward handler for The Old Church.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Quests/quests.xlsx
+++ b/resources/data-imports/Quests/quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="621">
   <si>
     <t>id</t>
   </si>
@@ -1737,6 +1737,51 @@
   </si>
   <si>
     <t>You come back to the building, you hold in your hand another journal. This one seems to belong to The Child. The Creator’s own Journal kept by The Poet. What secrets will you find with in it?&lt;br /&gt; &lt;br /&gt; The Soldiers Brother is no where to be seen. You sit on the counter and wait for him and read the Journal.&lt;br /&gt; &lt;br /&gt; “He couldn’t seem to handle the truth. I told him of his death today and he couldn't handle the truth.”&lt;br /&gt; &lt;br /&gt; You begin to read the only passage that seems to make sense, or isn’t scrambled by some kind of magic.&lt;br /&gt; &lt;br /&gt; “I told him he needed to ascend from this plane but he couldn’t let go of the the past, the love he lost, the mother he discovered to be among this land, the memories he creates are frozen in place and no matter how many winter nights pass and how many years begin and end, he refuses to accept the truth.&lt;br /&gt; &lt;br /&gt; The Child clings to the past disillusion and memories of a better time, a time he chose to end at his own hands. I have explained that his being here, his clinging to these memories and refusing to let go is slowly corrupting the land. He seems not to care.”&lt;br /&gt; &lt;br /&gt; How could one person do so much damage to a single world?&lt;br /&gt; &lt;br /&gt; “I see you found another book.” Comes a familiar voice.</t>
+  </si>
+  <si>
+    <t>Will it Hurt?</t>
+  </si>
+  <si>
+    <t>You return to the snow swept waste lands with a renewed mission in your heart, find a way to kill The Creator. His mother, The Ice Queen, she was easy enough to put down. She was a manifestation of pain, of grief – of never letting go.&lt;br /&gt; &lt;br /&gt; He is a corruption, a pain, a soulless husk of anger that cannot let go. He is the end of things, the beginning of others. He is the story you chase.&lt;br /&gt; &lt;br /&gt; You approach the church once again, you stare at its empty and dark windows.&lt;br /&gt; &lt;br /&gt; “You’re back child.”&lt;br /&gt; &lt;br /&gt; Mr. Whiskers walks up to you in the snow, his little paws leaving snow prints behind. You pick him up and he thanks you.&lt;br /&gt; &lt;br /&gt; “I know your task child. I know it all to well.”</t>
+  </si>
+  <si>
+    <t>Under the pine tree beside the church you and the cat sit in silence, watching the night snow fall on the ground. The flames burn I the small fire pit you have made, the warmth barley lifts the chill that haunts you.&lt;br /&gt; &lt;br /&gt; “Will it hurt?” The cat asks after a moment. You look over at him. “When you kill him that is. I was alone, darkness took me. Sickness kept him at bay. Haunting pain that lingers.”&lt;br /&gt; &lt;br /&gt; Corruption.&lt;br /&gt; &lt;br /&gt; You promise it wont hurt, that it you will free him, free him to free all of you.&lt;br /&gt; &lt;br /&gt; “A cleansing of the land? Will they all go away? Will there be any one left?”&lt;br /&gt; &lt;br /&gt; Will there?</t>
+  </si>
+  <si>
+    <t>The Father. AKA: Him</t>
+  </si>
+  <si>
+    <t>What will happen when you finally find a way to defeat The Creator? Can it even be done? Isn’t he beyond that of even The Poet, some kind of cosmic construct of magic? If The Poet cannot seem to lock him away or banish him or kill him, then what chance do you have?&lt;br /&gt; &lt;br /&gt; Can you raise your self to his level? The Creator’s that is? Can you become as powerful as him? Is that possible?&lt;br /&gt; &lt;br /&gt; No. You are a mortal. You are a single person. But Ascension…. What is it?</t>
+  </si>
+  <si>
+    <t>You found the cat napping under the tree, keeping out the snow. You’re jealous that his fur can keep the cold and the chill of the snow out.&lt;br /&gt; &lt;br /&gt; You ask him what Ascension is.&lt;br /&gt; &lt;br /&gt; “It’s an act where the lost soul fulfills what they came here to do, and moves on. They go off where ever souls go. To a happier place then where they come from I hope. They are the souls of the broken, the damaged, the lonely, the helpless.”&lt;br /&gt; &lt;br /&gt; You ask him how one ascends.&lt;br /&gt; &lt;br /&gt; “The Poet is suppose to guide the soul through their trials and tribulations. Through their grief and pain to the reality of their own choices. The reality they are dead. The poet believes that nothing is so broken it cannot be fixed. He has a deal with … Him.”&lt;br /&gt; &lt;br /&gt; The Creator?&lt;br /&gt; &lt;br /&gt; “No. Him.”&lt;br /&gt; &lt;br /&gt; God?&lt;br /&gt; &lt;br /&gt; “No. The Father.”&lt;br /&gt; &lt;br /&gt; Who is The Father? Is he secretly God?</t>
+  </si>
+  <si>
+    <t>The Errands and The Snow</t>
+  </si>
+  <si>
+    <t>“The Father, from what I know, is the incarnation of light. He is truth, substance, compassion and love. While the mother is Darkness, Pain and corruption. The Father made a deal with The Poet. He stated that for every broken soul The Poet Helps to Ascend to another plane of existence, one beyond the reach of The Mother, he would allow The Poet and his cosmic siblings to live in a world of their own creation.”&lt;br /&gt; &lt;br /&gt; So The Poet Created this world? His Siblings and him? The Ghosts of the past.&lt;br /&gt; &lt;br /&gt; “No, They came and took over a ruined world, one destroyed by war, by weapons of war that set the world back many millions of years. It was inhabited by people, elves, dwarves and many other types of beasts that roamed the world. Over thousands of years the world was shaped, formed and molded by The Poet and his siblings who you know as the various people you have interacted with.”&lt;br /&gt; &lt;br /&gt; The cat stands and stretches and walks out side.&lt;br /&gt; &lt;br /&gt; “I have business to do.”</t>
+  </si>
+  <si>
+    <t>You stand before the fallen enemies on the ground, they stalked the church and by extension you and Mr. Whiskers.&lt;br /&gt; &lt;br /&gt; You complete the tasks that Mr. Whiskers sets out before you. He dangles the key to the church before you, metaphorically that is. You wonder when he will let you into this place, it holds the answers you need. You know it does. Answers about the one this the Church knew about and kept under wraps: Ascension.&lt;br /&gt; &lt;br /&gt; You work your self till you are numb from the cold and tired from the labor. Your patience wares thin with the endless errands.</t>
+  </si>
+  <si>
+    <t>The Emerald Dream</t>
+  </si>
+  <si>
+    <t>You ask the cat when he is going to let you into the church. You almost demand the key you know he has. Where you have no idea. He is a cat after all – or as we put it now: A ghost of the past.&lt;br /&gt; &lt;br /&gt; “When you are ready for the truth of the situation.”&lt;br /&gt; &lt;br /&gt; Wait theirs more then what I have learned? Beyond The Father and all this pact talk and the whole facts this is all a construct being corrupted by a sad, lonely boy who committed suicide? What more could there be?</t>
+  </si>
+  <si>
+    <t>The cat looks at you.&lt;br /&gt; &lt;br /&gt; “The Church holds the path to The Emerald Dream. A place where The Emerald Prince lives. A man who is said to be a manifestation of magic, the creator of all magic. He is the man that holds the bounds of the realities and their planes in a stable position with in the fabric of time and space.”&lt;br /&gt; &lt;br /&gt; A man who is the father of magic. A man who holds the strings of realities in place, to stop them from drifting into the endless void. Trapping the residents in a desolate waste land of despair. You have heard these stories once before, long before – when you were a child. A man made of emeralds, a wizard in another dimension.&lt;br /&gt; &lt;br /&gt; You use to pretend to be him. It was a fable, a story. But what is these days.</t>
+  </si>
+  <si>
+    <t>The doors to The Old Church</t>
+  </si>
+  <si>
+    <t>You complete your tasks in silence the following day. Neither you or the cat speaks to each other for more then a few moments at a time.&lt;br /&gt; &lt;br /&gt; You are lost in your own thoughts and he is sleeping by the fire. Keeping warm while you freeze in the snow, slaughtering the beasts around the church, studying the exterior, memorizing it.&lt;br /&gt; &lt;br /&gt; You see the shadows dance in your own mind, on the landscape, in the snow.</t>
+  </si>
+  <si>
+    <t>You arrive back at the small camp and the cat rises and stretches.&lt;br /&gt; &lt;br /&gt; “Into the church you go. The magic of the barrier has been lifted and you might need this to enter it.”&lt;br /&gt; &lt;br /&gt; He produces a Christmas Tree Light Bulb.&lt;br /&gt; &lt;br /&gt; “Holding this will allow you to enter the building. With out it, you would be torn apart by the shadows of the past. The ones you saw dancing earlier.”&lt;br /&gt; &lt;br /&gt; You walk through the church doors and into the main area. It is silent, it is dark. The stories of The Emerald Prince must be here ...</t>
   </si>
   <si>
     <t>Defeating The Queen</t>
@@ -2172,7 +2217,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AF129"/>
+  <dimension ref="A1:AF134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -7258,7 +7303,7 @@
     </row>
     <row r="122" spans="1:32">
       <c r="A122">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B122" t="s">
         <v>574</v>
@@ -7266,76 +7311,61 @@
       <c r="C122" t="s">
         <v>471</v>
       </c>
-      <c r="D122" t="s">
+      <c r="E122" t="s">
+        <v>559</v>
+      </c>
+      <c r="M122">
+        <v>175</v>
+      </c>
+      <c r="N122">
+        <v>75</v>
+      </c>
+      <c r="O122">
+        <v>2000</v>
+      </c>
+      <c r="P122">
+        <v>100</v>
+      </c>
+      <c r="T122" t="s">
+        <v>470</v>
+      </c>
+      <c r="Z122" t="s">
         <v>575</v>
       </c>
-      <c r="E122" t="s">
-        <v>543</v>
-      </c>
-      <c r="H122">
-        <v>125</v>
-      </c>
-      <c r="I122">
-        <v>25000</v>
-      </c>
-      <c r="M122">
-        <v>75</v>
-      </c>
-      <c r="N122">
-        <v>10</v>
-      </c>
-      <c r="O122">
-        <v>200</v>
-      </c>
-      <c r="P122">
-        <v>100</v>
-      </c>
-      <c r="S122">
-        <v>1</v>
-      </c>
-      <c r="Z122" t="s">
+      <c r="AA122" t="s">
         <v>576</v>
       </c>
-      <c r="AA122" t="s">
-        <v>577</v>
-      </c>
-      <c r="AB122" t="s">
-        <v>575</v>
-      </c>
       <c r="AC122" t="s">
-        <v>543</v>
+        <v>559</v>
       </c>
       <c r="AD122">
         <v>4</v>
       </c>
+      <c r="AE122" t="s">
+        <v>471</v>
+      </c>
+      <c r="AF122">
+        <v>5</v>
+      </c>
     </row>
     <row r="123" spans="1:32">
       <c r="A123">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="B123" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C123" t="s">
         <v>471</v>
       </c>
-      <c r="G123" t="s">
-        <v>579</v>
-      </c>
-      <c r="H123">
-        <v>125</v>
-      </c>
-      <c r="I123">
-        <v>5000</v>
-      </c>
       <c r="M123">
+        <v>175</v>
+      </c>
+      <c r="N123">
         <v>75</v>
       </c>
-      <c r="N123">
-        <v>10</v>
-      </c>
       <c r="O123">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="P123">
         <v>100</v>
@@ -7344,171 +7374,192 @@
         <v>574</v>
       </c>
       <c r="Z123" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="AA123" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="AD123">
         <v>4</v>
       </c>
+      <c r="AE123" t="s">
+        <v>471</v>
+      </c>
+      <c r="AF123">
+        <v>10</v>
+      </c>
     </row>
     <row r="124" spans="1:32">
       <c r="A124">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B124" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C124" t="s">
         <v>471</v>
       </c>
-      <c r="G124" t="s">
-        <v>583</v>
-      </c>
-      <c r="H124">
-        <v>125</v>
-      </c>
-      <c r="I124">
-        <v>10000</v>
-      </c>
       <c r="M124">
+        <v>175</v>
+      </c>
+      <c r="N124">
         <v>75</v>
       </c>
-      <c r="N124">
-        <v>10</v>
+      <c r="O124">
+        <v>2000</v>
       </c>
       <c r="P124">
         <v>100</v>
       </c>
       <c r="T124" t="s">
-        <v>578</v>
-      </c>
-      <c r="U124" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="Z124" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="AA124" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="AD124">
         <v>4</v>
       </c>
+      <c r="AE124" t="s">
+        <v>471</v>
+      </c>
+      <c r="AF124">
+        <v>15</v>
+      </c>
     </row>
     <row r="125" spans="1:32">
       <c r="A125">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B125" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="C125" t="s">
         <v>471</v>
       </c>
-      <c r="G125" t="s">
-        <v>588</v>
-      </c>
-      <c r="H125">
-        <v>125</v>
-      </c>
-      <c r="I125">
+      <c r="M125">
+        <v>175</v>
+      </c>
+      <c r="N125">
+        <v>75</v>
+      </c>
+      <c r="O125">
         <v>2000</v>
       </c>
-      <c r="O125">
-        <v>200</v>
-      </c>
       <c r="P125">
         <v>100</v>
       </c>
       <c r="T125" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="Z125" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="AA125" t="s">
-        <v>590</v>
+        <v>585</v>
+      </c>
+      <c r="AD125">
+        <v>4</v>
+      </c>
+      <c r="AE125" t="s">
+        <v>471</v>
+      </c>
+      <c r="AF125">
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:32">
       <c r="A126">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B126" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="C126" t="s">
         <v>471</v>
       </c>
-      <c r="G126" t="s">
-        <v>592</v>
-      </c>
-      <c r="H126">
-        <v>125</v>
-      </c>
-      <c r="I126">
-        <v>20000</v>
+      <c r="M126">
+        <v>175</v>
+      </c>
+      <c r="N126">
+        <v>75</v>
       </c>
       <c r="O126">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="P126">
         <v>100</v>
       </c>
       <c r="T126" t="s">
+        <v>583</v>
+      </c>
+      <c r="Z126" t="s">
         <v>587</v>
       </c>
-      <c r="Z126" t="s">
-        <v>593</v>
-      </c>
       <c r="AA126" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="AD126">
         <v>4</v>
       </c>
+      <c r="AE126" t="s">
+        <v>471</v>
+      </c>
+      <c r="AF126">
+        <v>25</v>
+      </c>
     </row>
     <row r="127" spans="1:32">
       <c r="A127">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B127" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="C127" t="s">
-        <v>428</v>
-      </c>
-      <c r="G127" t="s">
-        <v>596</v>
+        <v>471</v>
+      </c>
+      <c r="D127" t="s">
+        <v>590</v>
+      </c>
+      <c r="E127" t="s">
+        <v>543</v>
       </c>
       <c r="H127">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="I127">
         <v>25000</v>
       </c>
       <c r="M127">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N127">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="O127">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P127">
         <v>100</v>
       </c>
-      <c r="T127" t="s">
+      <c r="S127">
+        <v>1</v>
+      </c>
+      <c r="Z127" t="s">
         <v>591</v>
       </c>
-      <c r="Z127" t="s">
-        <v>597</v>
-      </c>
       <c r="AA127" t="s">
-        <v>598</v>
+        <v>592</v>
+      </c>
+      <c r="AB127" t="s">
+        <v>590</v>
+      </c>
+      <c r="AC127" t="s">
+        <v>543</v>
       </c>
       <c r="AD127">
         <v>4</v>
@@ -7516,40 +7567,43 @@
     </row>
     <row r="128" spans="1:32">
       <c r="A128">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B128" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="C128" t="s">
         <v>471</v>
       </c>
-      <c r="E128" t="s">
-        <v>595</v>
-      </c>
       <c r="G128" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="H128">
         <v>125</v>
       </c>
       <c r="I128">
-        <v>20000</v>
+        <v>5000</v>
+      </c>
+      <c r="M128">
+        <v>75</v>
+      </c>
+      <c r="N128">
+        <v>10</v>
+      </c>
+      <c r="O128">
+        <v>200</v>
       </c>
       <c r="P128">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="T128" t="s">
-        <v>574</v>
+        <v>589</v>
       </c>
       <c r="Z128" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="AA128" t="s">
-        <v>602</v>
-      </c>
-      <c r="AC128" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="AD128">
         <v>4</v>
@@ -7557,33 +7611,235 @@
     </row>
     <row r="129" spans="1:32">
       <c r="A129">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B129" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="C129" t="s">
         <v>471</v>
       </c>
+      <c r="G129" t="s">
+        <v>598</v>
+      </c>
       <c r="H129">
         <v>125</v>
       </c>
       <c r="I129">
+        <v>10000</v>
+      </c>
+      <c r="M129">
+        <v>75</v>
+      </c>
+      <c r="N129">
+        <v>10</v>
+      </c>
+      <c r="P129">
+        <v>100</v>
+      </c>
+      <c r="T129" t="s">
+        <v>593</v>
+      </c>
+      <c r="U129" t="s">
+        <v>599</v>
+      </c>
+      <c r="Z129" t="s">
+        <v>600</v>
+      </c>
+      <c r="AA129" t="s">
+        <v>601</v>
+      </c>
+      <c r="AD129">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:32">
+      <c r="A130">
+        <v>121</v>
+      </c>
+      <c r="B130" t="s">
+        <v>602</v>
+      </c>
+      <c r="C130" t="s">
+        <v>471</v>
+      </c>
+      <c r="G130" t="s">
+        <v>603</v>
+      </c>
+      <c r="H130">
+        <v>125</v>
+      </c>
+      <c r="I130">
+        <v>2000</v>
+      </c>
+      <c r="O130">
+        <v>200</v>
+      </c>
+      <c r="P130">
+        <v>100</v>
+      </c>
+      <c r="T130" t="s">
+        <v>597</v>
+      </c>
+      <c r="Z130" t="s">
+        <v>604</v>
+      </c>
+      <c r="AA130" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="131" spans="1:32">
+      <c r="A131">
+        <v>122</v>
+      </c>
+      <c r="B131" t="s">
+        <v>606</v>
+      </c>
+      <c r="C131" t="s">
+        <v>471</v>
+      </c>
+      <c r="G131" t="s">
+        <v>607</v>
+      </c>
+      <c r="H131">
+        <v>125</v>
+      </c>
+      <c r="I131">
+        <v>20000</v>
+      </c>
+      <c r="O131">
+        <v>200</v>
+      </c>
+      <c r="P131">
+        <v>100</v>
+      </c>
+      <c r="T131" t="s">
+        <v>602</v>
+      </c>
+      <c r="Z131" t="s">
+        <v>608</v>
+      </c>
+      <c r="AA131" t="s">
+        <v>609</v>
+      </c>
+      <c r="AD131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:32">
+      <c r="A132">
+        <v>123</v>
+      </c>
+      <c r="B132" t="s">
+        <v>610</v>
+      </c>
+      <c r="C132" t="s">
+        <v>428</v>
+      </c>
+      <c r="G132" t="s">
+        <v>611</v>
+      </c>
+      <c r="H132">
+        <v>100</v>
+      </c>
+      <c r="I132">
+        <v>25000</v>
+      </c>
+      <c r="M132">
+        <v>25</v>
+      </c>
+      <c r="N132">
+        <v>2</v>
+      </c>
+      <c r="O132">
+        <v>150</v>
+      </c>
+      <c r="P132">
+        <v>100</v>
+      </c>
+      <c r="T132" t="s">
+        <v>606</v>
+      </c>
+      <c r="Z132" t="s">
+        <v>612</v>
+      </c>
+      <c r="AA132" t="s">
+        <v>613</v>
+      </c>
+      <c r="AD132">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:32">
+      <c r="A133">
+        <v>124</v>
+      </c>
+      <c r="B133" t="s">
+        <v>614</v>
+      </c>
+      <c r="C133" t="s">
+        <v>471</v>
+      </c>
+      <c r="E133" t="s">
+        <v>610</v>
+      </c>
+      <c r="G133" t="s">
+        <v>615</v>
+      </c>
+      <c r="H133">
+        <v>125</v>
+      </c>
+      <c r="I133">
+        <v>20000</v>
+      </c>
+      <c r="P133">
+        <v>200</v>
+      </c>
+      <c r="T133" t="s">
+        <v>589</v>
+      </c>
+      <c r="Z133" t="s">
+        <v>616</v>
+      </c>
+      <c r="AA133" t="s">
+        <v>617</v>
+      </c>
+      <c r="AC133" t="s">
+        <v>610</v>
+      </c>
+      <c r="AD133">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:32">
+      <c r="A134">
+        <v>125</v>
+      </c>
+      <c r="B134" t="s">
+        <v>618</v>
+      </c>
+      <c r="C134" t="s">
+        <v>471</v>
+      </c>
+      <c r="H134">
+        <v>125</v>
+      </c>
+      <c r="I134">
         <v>30000</v>
       </c>
-      <c r="P129">
+      <c r="P134">
         <v>500</v>
       </c>
-      <c r="T129" t="s">
-        <v>599</v>
-      </c>
-      <c r="Z129" t="s">
-        <v>604</v>
-      </c>
-      <c r="AA129" t="s">
-        <v>605</v>
-      </c>
-      <c r="AD129">
+      <c r="T134" t="s">
+        <v>614</v>
+      </c>
+      <c r="Z134" t="s">
+        <v>619</v>
+      </c>
+      <c r="AA134" t="s">
+        <v>620</v>
+      </c>
+      <c r="AD134">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding a new event for faction loyalty
</commit_message>
<xml_diff>
--- a/resources/data-imports/Quests/quests.xlsx
+++ b/resources/data-imports/Quests/quests.xlsx
@@ -11165,8 +11165,8 @@
       <c r="Q193">
         <v>2000000</v>
       </c>
-      <c r="T193">
-        <v>1</v>
+      <c r="U193" t="s">
+        <v>845</v>
       </c>
       <c r="AA193" t="s">
         <v>851</v>
@@ -11227,11 +11227,11 @@
       <c r="Q194">
         <v>200000</v>
       </c>
-      <c r="T194">
-        <v>1</v>
+      <c r="U194" t="s">
+        <v>849</v>
       </c>
       <c r="Y194">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA194" t="s">
         <v>855</v>

</xml_diff>

<commit_message>
Updating and various fixes to building upgrades/repairing.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Quests/quests.xlsx
+++ b/resources/data-imports/Quests/quests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="911">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -3031,8 +3031,8 @@
   </sheetPr>
   <dimension ref="A1:AG206"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U82" activeCellId="0" sqref="U82"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD1" activeCellId="0" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6478,6 +6478,9 @@
       <c r="Q82" s="1" t="n">
         <v>200</v>
       </c>
+      <c r="U82" s="1" t="s">
+        <v>401</v>
+      </c>
       <c r="Z82" s="1" t="s">
         <v>410</v>
       </c>

</xml_diff>

<commit_message>
Minor fixes to the way the ice plane event works
</commit_message>
<xml_diff>
--- a/resources/data-imports/Quests/quests.xlsx
+++ b/resources/data-imports/Quests/quests.xlsx
@@ -2408,7 +2408,7 @@
     <t>The running theme</t>
   </si>
   <si>
-    <t>Musty Childs Teddy bare</t>
+    <t>Musty Childs Teddy Bear</t>
   </si>
   <si>
     <t>It's been several days since you parted ways with the Lonely Red Hawk Soldier, initially perceived as a mere apparition of the man interred in this very grave, only to discover that he was indeed a deceased Red Hawk &lt;br /&gt; Soldier, slain by his own desire of flesh.&lt;br /&gt; &lt;br /&gt; Death casts its long shadow over this realm, as it does across all planes of existence. Briefly, you ponder whether death serves as the central motif of this reality, as your own life seems entwined with a recurring theme &lt;br /&gt; of death. Moving through the narratives of others, seeking answers, only to find yourself inundated with information that has thus far led you down a path fraught with more death and desolation.&lt;br /&gt; &lt;br /&gt; In the past few days, you've lingered near the grave, setting up camp not far away. The man who introduced himself as the Grave Digger tends to this solitary resting place, although a grieving brother would have been a &lt;br /&gt; more fitting moniker. Yet another individual, another entity unable to release their grip on loss.&lt;br /&gt; &lt;br /&gt; It seems yet another theme has revealed itself.</t>
@@ -8450,7 +8450,7 @@
         <v>595</v>
       </c>
       <c r="AE125">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:33">
@@ -8482,7 +8482,7 @@
         <v>599</v>
       </c>
       <c r="AE126">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:33">
@@ -8514,7 +8514,7 @@
         <v>603</v>
       </c>
       <c r="AE127">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:33">
@@ -8546,7 +8546,7 @@
         <v>606</v>
       </c>
       <c r="AE128">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:33">
@@ -8596,7 +8596,7 @@
         <v>608</v>
       </c>
       <c r="AE129">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:33">
@@ -8637,7 +8637,7 @@
         <v>615</v>
       </c>
       <c r="AE130">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:33">
@@ -8681,7 +8681,7 @@
         <v>604</v>
       </c>
       <c r="AE131">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:33">
@@ -8722,7 +8722,7 @@
         <v>623</v>
       </c>
       <c r="AE132">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:33">
@@ -8772,7 +8772,7 @@
         <v>627</v>
       </c>
       <c r="AE133">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:33">
@@ -8819,7 +8819,7 @@
         <v>613</v>
       </c>
       <c r="AE134">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135" spans="1:33">
@@ -8863,7 +8863,7 @@
         <v>637</v>
       </c>
       <c r="AE135">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:33">
@@ -8913,7 +8913,7 @@
         <v>643</v>
       </c>
       <c r="AE136">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:33">
@@ -8960,7 +8960,7 @@
         <v>647</v>
       </c>
       <c r="AE137">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:33">
@@ -9010,7 +9010,7 @@
         <v>650</v>
       </c>
       <c r="AE138">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:33">
@@ -9051,7 +9051,7 @@
         <v>658</v>
       </c>
       <c r="AE139">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:33">
@@ -9095,7 +9095,7 @@
         <v>663</v>
       </c>
       <c r="AE140">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:33">
@@ -9139,7 +9139,7 @@
         <v>668</v>
       </c>
       <c r="AE141">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:33">
@@ -9183,7 +9183,7 @@
         <v>672</v>
       </c>
       <c r="AE142">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:33">
@@ -9230,7 +9230,7 @@
         <v>669</v>
       </c>
       <c r="AE143">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:33">
@@ -9271,7 +9271,7 @@
         <v>679</v>
       </c>
       <c r="AE144">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:33">
@@ -9312,7 +9312,7 @@
         <v>682</v>
       </c>
       <c r="AE145">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:33">
@@ -9359,7 +9359,7 @@
         <v>644</v>
       </c>
       <c r="AE146">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:33">
@@ -9403,7 +9403,7 @@
         <v>689</v>
       </c>
       <c r="AE147">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:33">
@@ -9444,7 +9444,7 @@
         <v>692</v>
       </c>
       <c r="AE148">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:33">
@@ -9526,7 +9526,7 @@
         <v>680</v>
       </c>
       <c r="AE150">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF150" t="s">
         <v>592</v>
@@ -9567,7 +9567,7 @@
         <v>700</v>
       </c>
       <c r="AE151">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF151" t="s">
         <v>592</v>
@@ -9608,7 +9608,7 @@
         <v>703</v>
       </c>
       <c r="AE152">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF152" t="s">
         <v>592</v>
@@ -9649,7 +9649,7 @@
         <v>706</v>
       </c>
       <c r="AE153">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF153" t="s">
         <v>592</v>
@@ -9693,7 +9693,7 @@
         <v>710</v>
       </c>
       <c r="AE154">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF154" t="s">
         <v>592</v>
@@ -9752,7 +9752,7 @@
         <v>664</v>
       </c>
       <c r="AE155">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156" spans="1:33">
@@ -9796,7 +9796,7 @@
         <v>718</v>
       </c>
       <c r="AE156">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:33">
@@ -9840,7 +9840,7 @@
         <v>723</v>
       </c>
       <c r="AE157">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:33">
@@ -9913,7 +9913,7 @@
         <v>731</v>
       </c>
       <c r="AE159">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160" spans="1:33">
@@ -9957,7 +9957,7 @@
         <v>735</v>
       </c>
       <c r="AE160">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:33">
@@ -9998,7 +9998,7 @@
         <v>732</v>
       </c>
       <c r="AE161">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" spans="1:33">
@@ -10033,7 +10033,7 @@
         <v>742</v>
       </c>
       <c r="AE162">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:33">

</xml_diff>

<commit_message>
Added new quests for the raid
</commit_message>
<xml_diff>
--- a/resources/data-imports/Quests/quests.xlsx
+++ b/resources/data-imports/Quests/quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1062">
   <si>
     <t>id</t>
   </si>
@@ -3132,6 +3132,75 @@
   </si>
   <si>
     <t>You return with the imperfect gold bar. Standing before the Dungeon Master, he speaks in a hushed and wise tone.&lt;br /&gt; &lt;br /&gt; "You give me a gift for the ages. Now, I shall give you what you seek."&lt;br /&gt; &lt;br /&gt; He unfolds a scroll and begins to read:&lt;br /&gt; &lt;br /&gt; "By the laws of the planes and the judges that live, you are now permitted to manage your kingdom's gold bars through the capital city."&lt;br /&gt; &lt;br /&gt; He rolls the scroll up and looks at you.&lt;br /&gt; &lt;br /&gt; "That's that."</t>
+  </si>
+  <si>
+    <t>A locket of her hair</t>
+  </si>
+  <si>
+    <t>The Frozen King</t>
+  </si>
+  <si>
+    <t>Locket of her hair</t>
+  </si>
+  <si>
+    <t>Necklace of silver</t>
+  </si>
+  <si>
+    <t>You awaken in the familiar, worn interior of a house. The warmth of a crackling fire envelops you, easing the chill that lingers in your bones. You sit up slowly, scanning the room until your eyes land on Mrs. Piper, who sits serenely by the hearth, her purrs blending with the fire's gentle pops.&lt;br /&gt; &lt;br /&gt; “Easy now,” she says in that small, squeaky voice that has grown so familiar. She rises and pads over, rubbing her head against your arm as if reassuring you of your safety. You stroke her absentmindedly, trying to piece together how you ended up here. The last thing you remember is the icy sting of the armored man's attack, but everything after that is a blur.&lt;br /&gt; &lt;br /&gt; “You almost died,” she says after a moment, her tone matter-of-fact. The words jar you, and you turn to her with wide eyes.&lt;br /&gt; &lt;br /&gt; “Almost died?” you repeat, trying to comprehend. You ask her for details, but she only flicks her tail and moves a few paces away. She stretches luxuriously before resuming her grooming, as if your brush with death is no more significant than a passing breeze.&lt;br /&gt; &lt;br /&gt; “Yes, child,” she says, pausing mid-lick. “Almost died. What’s so hard to understand about that?”&lt;br /&gt; &lt;br /&gt; The entire situation, you tell her. The armored man, the battle, the bitter wind—it all seems surreal. &lt;br /&gt; &lt;br /&gt; She sighs, fixing you with an unblinking stare. “Look, you’re not ready to face him yet. You need something more, something precious to him, something that binds him to his past. Hers, his, their child’s.”&lt;br /&gt; &lt;br /&gt; Confusion knots your brow. What could you need beyond your magic, your weapons, and the sheer will to fight?&lt;br /&gt; &lt;br /&gt; “You need these items combined to face him, to confront the truth, and ultimately to kill him,” Mrs. Piper continues, her eyes narrowing as if challenging you to grasp the gravity of her words.&lt;br /&gt; &lt;br /&gt; “A locket of hair,” she says, breaking the silence. “Find me that—a locket of her hair. I don’t know where it is, but one of his minions might have it.”&lt;br /&gt; &lt;br /&gt; A locket of hair? The idea strikes you as absurd. Could such a simple thing really be the key to defeating him? Your mind races with questions, but Mrs. Piper’s gaze remains steady, leaving you with no doubt that this quest is necessary.</t>
+  </si>
+  <si>
+    <t>After a grueling battle, you return, battered and exhausted, holding the prize of your efforts—a small, tarnished locket containing delicate strands of golden hair. You set it down on the table, and Mrs. Piper leaps up to inspect it. She paws at the locket, sniffs it curiously, and even attempts to bite it gently. Her actions puzzle you, and you arch an eyebrow in question.&lt;br /&gt; &lt;br /&gt; “This is it,” she confirms, her voice soft but certain. “A locket of her hair. He loved her deeply, cherished her memory, what she represented: simpler, better times.”&lt;br /&gt; &lt;br /&gt; You watch her, the realization settling over you like a weight. This trinket, so small and seemingly insignificant, holds a deep emotional power. You wonder aloud what else you’ll need. What could possibly embody him? And what of their son—what piece of his essence must you find?&lt;br /&gt; &lt;br /&gt; Mrs. Piper’s eyes gleam with a knowing light. “Take this necklace to Mr. Whiskers.” She nudges a delicate silver chain across the table. It slides off the edge and clatters to the floor. Before she can pounce on it for play, you stoop and pick it up. It feels cool in your hand, deceptively simple.&lt;br /&gt; &lt;br /&gt; “He will give you something of the father’s,” she continues, her tone more serious now. “Bring it back, and we’ll need only one more thing. One last piece to take to him, The Frozen King. With these items and another, you can forge a magical tool capable of ending him, destroying him once and for all.”&lt;br /&gt; &lt;br /&gt; Her words leave you with a sense of anticipation, mingled with frustration. She pads back to the fire, curling up in its warmth, while you study the necklace in your hand. Its silver gleam reminds you of the armor The Enchanted Snowman once wore, of his voice that chilled your very soul, of his command to face him.&lt;br /&gt; &lt;br /&gt; You replay that encounter in your mind: how you readied yourself, only to end up here, defeated but alive. Mrs. Piper’s insistence echoes in your thoughts—why were these objects necessary? Why was your magic, your willpower, not enough? What hidden power lay in these simple keepsakes that made them essential to facing him? Doubts nag at you, but with a deep breath, you resolve to see this quest through to its end.</t>
+  </si>
+  <si>
+    <t>A clock for a cat</t>
+  </si>
+  <si>
+    <t>Golden Pocket Watch</t>
+  </si>
+  <si>
+    <t>Black Fur Coat</t>
+  </si>
+  <si>
+    <t>You return to the abandoned village, its familiar desolation punctuated by the whispers of the wind and the groan of old, weathered wood. The house where Mr. Whiskers resides stands as it did before, a silent sentinel in this forsaken place. As you step inside, a purr greets you, followed by a meow, and the little cat bounds out from another room, eyes alight with anticipation.&lt;br /&gt; &lt;br /&gt; “Hello there! Have you come to play?” His question is innocent, yet you feel the weight of your mission. You explain quickly that Mrs. Piper sent you, that you carry something significant, and that he, too, might hold a piece needed for this battle against The Frozen King. You add, with a tinge of frustration, that you still don’t understand why you alone aren’t enough—why these items are essential when you are prepared to fight with all you have.&lt;br /&gt; &lt;br /&gt; Mr. Whiskers listens, his expression thoughtful, his tail flicking behind him. “His magic is too strong, child,” he says, a rare seriousness in his voice. “You are not on even ground with him as you are with others. His pain is his shield, his loss a haunting specter, and his longing for his wife—his most potent weapon. You must break him, make him see the truth, and only then will you have the chance to strike.”&lt;br /&gt; &lt;br /&gt; You swallow hard and ask if defeating The Frozen King will lift the icy curse that blankets the land, that both he and his wife perpetuate.&lt;br /&gt; &lt;br /&gt; Mr. Whiskers’ eyes narrow, filled with an ancient sadness. “I am afraid not, child. The Creator sustains this place, frozen in its torment. Only by confronting and putting him down can you ever hope to mend this world, if it is even possible to heal such wounds.”&lt;br /&gt; &lt;br /&gt; The realization makes your chest tighten. How could you ever face The Creator? Perhaps it would require the same approach as The Frozen King—a methodical gathering of pieces to break through the defenses of pain and memory. You shake your head to clear it, focusing on the task at hand.&lt;br /&gt; &lt;br /&gt; You show Mr. Whiskers the simple silver necklace Mrs. Piper had given you and ask if he has anything that can be combined with it and the locket of hair to create the weapon that will help break The Frozen King’s power.&lt;br /&gt; &lt;br /&gt; “I do,” he admits, but a playful glint returns to his eyes. “But I also enjoy seeing time—time that has passed, time that is present, and time that has yet to come. Can you bring that to me?”&lt;br /&gt; &lt;br /&gt; You blink at him, puzzled. Time? What could he mean? A clock?</t>
+  </si>
+  <si>
+    <t>The plains are stained with the remnants of your battle, the air still vibrating with echoes of your magic. The creature, now motionless, lies before you as you catch your breath. Among its torn belongings, you spot a pocket watch, glinting dully in the faint light. You pick it up and turn it over in your hand, its surface cold and worn. When you open it, the hands still tick, pointing to four-forty. &lt;br /&gt; &lt;br /&gt; Why would Mr. Whiskers, a cat bound to the echoes of memory and mischief, care about such a thing? Why would he need to see the passage of time? A chill creeps down your spine as you wonder if this has significance beyond the simple whimsy he presented. You shake the thought away and make your way back to the abandoned house.&lt;br /&gt; &lt;br /&gt; The creaking floorboards announce your return as you push the door open. Mr. Whiskers’ eyes gleam as he spies the watch in your hand. “Ah yes, I can now… Wait…” He narrows his eyes, seemingly puzzled. “I can’t tell time. What time is it?” &lt;br /&gt; &lt;br /&gt; You glance down. The watch reads six-thirty. &lt;br /&gt; &lt;br /&gt; “Six-thirty?! I haven’t been fed yet!” His voice is indignant, but you remind him of his state—that he is long dead, unable to feel hunger. &lt;br /&gt; &lt;br /&gt; “Right you are, child. Right you are!” His demeanor shifts again to a playful bounce as he leaps from the table and disappears into the shadows of another room. Moments later, his purr echoes back, and he emerges, carrying something in his mouth. He drops it at your feet with a soft thud.&lt;br /&gt; &lt;br /&gt; You reach down and pick it up—a coat, fur-lined, and heavier than it looks. It exudes a peculiar warmth despite the chill in the air. You eye Mr. Whiskers, puzzled at how he managed to carry it with such ease.&lt;br /&gt; &lt;br /&gt; “This is what Mrs. Piper needs,” he says with a flick of his tail, batting at the watch on the table as though it were a toy.&lt;br /&gt; &lt;br /&gt; Before you leave, questions bubble in your mind. You ask how The Frozen King broke free from his snowman-like appearance.&lt;br /&gt; &lt;br /&gt; “Oh, I don’t know, child,” Mr. Whiskers says, his paw now tapping the ticking watch absently. “I do know he is made of the same magic that binds this place. He was created by Trix and The Poet, and is a corruption steeped in pain. The rest, well, you’d have to ask him yourself.”&lt;br /&gt; &lt;br /&gt; Of course, you think. You would have to confront him to learn more. But another question lingers. You ask Mr. Whiskers if he ever feels lonely, if he misses The Creator, and why he isn’t consumed by pain like the others.&lt;br /&gt; &lt;br /&gt; The cat pauses, his gaze drifting into the middle distance as if looking at something beyond your sight. “Because I am at peace with my death. I lived a long, full life, a happy life. The Creator loved me from the day he brought me home to long after his own death. My memory, my existence, is a sliver of humanity that keeps him tethered.”&lt;br /&gt; &lt;br /&gt; A sliver of humanity. The words settle heavily in your mind. Could The Frozen King, too, possess such a thing buried within his tortured existence? The thought flickers like a hesitant flame before you dismiss it, but it lingers, refusing to be fully extinguished.</t>
+  </si>
+  <si>
+    <t>Broken Memories</t>
+  </si>
+  <si>
+    <t>Dust of broken memories</t>
+  </si>
+  <si>
+    <t>Family Photo</t>
+  </si>
+  <si>
+    <t>The room is quiet save for the low crackle of the fire and Mrs. Piper's content purring as she curls deeper into the jacket. You stand by the window, eyes scanning the darkened landscape beyond, where the wind lashes the trees and whispers of a coming storm. The sky is dark, heavy with clouds that seem to press down on the world like an omen. The silence grows thick between you and the small cat until you turn and break it with a question.&lt;br /&gt; &lt;br /&gt; “What’s next? What other item do I need?” Your voice is steady, masking the simmering unease that tightens your chest.&lt;br /&gt; &lt;br /&gt; Mrs. Piper’s eyes glint in the dim light as she lifts her head, ears twitching. “A family photo,” she states, her voice light and matter-of-fact, but there’s a seriousness beneath it. &lt;br /&gt; &lt;br /&gt; You frown. A family photo? Why would that hold any power? Before you can ask, she explains, “The Frozen King, known as The Father, cherished his family. With the photo, the locket, and the coat, I can use the magic of this place to create something special for you. Something you can use on him, or at least on an aspect of him.”&lt;br /&gt; &lt;br /&gt; “An aspect?” you repeat, trying to grasp the meaning. But she offers no further explanation, only a soft, evasive blink.&lt;br /&gt; &lt;br /&gt; The question of how you escaped from The Frozen King’s clutches earlier bubbles up again. “How did I manage to escape him before?” you ask, your voice edged with doubt.&lt;br /&gt; &lt;br /&gt; Mrs. Piper's whiskers twitch, and a small smile curves her mouth. “You didn’t. I whisked you away. I brought you here.”&lt;br /&gt; &lt;br /&gt; “By magic?” The disbelief is evident in your tone, though part of you already knows the answer.&lt;br /&gt; &lt;br /&gt; “Of course,” she replies, tilting her head with a knowing look. “Everything in this world, everything you have encountered is either dead, a memory, or magic. I am magic. I am also a memory. But I am not dead.” Her voice lifts with a note of pride at the last statement.&lt;br /&gt; &lt;br /&gt; Her words stir memories of what Mr. Whiskers told you earlier about The Creator, how he held onto a sliver of humanity. You tell her about what the cat said, and the question that gnaws at you resurfaces: “Does The Frozen King have a sliver of humanity too? If so, how can he be so consumed by pain?”&lt;br /&gt; &lt;br /&gt; Mrs. Piper’s eyes narrow thoughtfully, her fur catching the orange glow of the fire. “Everyone, even the darkest of creatures, has a sliver of humanity. They are all tied to The Creator. Whiskers is correct—he is the last vestige of humanity The Creator holds onto, a memory of love, just like me.”&lt;br /&gt; &lt;br /&gt; The idea spins in your mind. If these remnants of humanity exist, could they be used against the King? Could they be turned into weapons or shields, something more powerful than brute strength or raw magic?&lt;br /&gt; &lt;br /&gt; The thought takes root, growing as you step back into the cold night, determination building in your chest. The storm gathers overhead, but your path is set. You have one more piece to find—a family photo that may hold the key to confronting The Frozen King.</t>
+  </si>
+  <si>
+    <t>You found a photo, one with a broken frame and busted glass, but through that you can see a child, a mother and a father, loving, smiling and happy. Holding it makes you feel happy, makes you wonder how this world became so corrupted, so pain filled and hate filled.&lt;br /&gt; &lt;br /&gt; You are left wondering The Poet didn’t do more to help The Creator, to stop all of this. You wonder if The Creator had this, if the world would have shattered in the way every one sais it has. You can’t say for sure but you grew up in this world, in a place where parents and adults talked about other places, like The Labyrinth or Even Shadow Planes.&lt;br /&gt; &lt;br /&gt; As you wonder this you take it back to Mrs. Piper. You show her the photo and ask her how everything got so broken.&lt;br /&gt; &lt;br /&gt; “It’s simple child. Pain.” She looks at the image you place on the table, and sniffs it.&lt;br /&gt; &lt;br /&gt; “Pain is what caused all of this, Pain caused The Shattering, pain caused The Frozen King to be who he is. Pain, its the root of all of this.”&lt;br /&gt; &lt;br /&gt; You wonder how to cure all this pain and ask her if it can be.&lt;br /&gt; &lt;br /&gt; “Eventually, but right now we have a bigger issue, The Frozen King is trying to take more of a hold on this plane, you must take the item I give you and use it on an aspect of him.”&lt;br /&gt; &lt;br /&gt; With in a moment the coat, the locket and the photo disappear and before you on the table is a vile, a vile of what looks like dust. You ask her what this is.&lt;br /&gt; &lt;br /&gt; “This, is a dust of broken memories. You sprinkle it on the aspect of him and it will cause his mind to shatter, allowing you to use everything you have to take him down. But this dust alone isn’t all that will be needed, you will need a shield. A shield to deflect his rage. Rage you have felt through the ice that whips through the wind.”&lt;br /&gt; &lt;br /&gt; You take the vile in your hand and look at it. It radiates with warmth. You look at her and give her a quick pet, she truly is a link to a sliver of humanity, much like Mr. Whiskers is, or was. A tear falls down your face.</t>
+  </si>
+  <si>
+    <t>Faceing the king</t>
+  </si>
+  <si>
+    <t>Shield of Hope</t>
+  </si>
+  <si>
+    <t>The old lot is silent but for the creaking of lifeless branches swaying in the wind. The dead trees, once picked for festive joy, now stand as hollow, brittle reminders of lost warmth. Snow crunches under your boots as you approach, eyes locked on the towering figure of The Frozen King beside the snowman. His silhouette is unmoving, his presence a void that seems to draw in the cold and amplify it.&lt;br /&gt; &lt;br /&gt; “Face me!” Your voice cuts through the icy air, sharp and commanding. But he doesn’t stir. The wind whips around you, carrying sharp shards of ice that sting your exposed skin. You pull your cloak tighter, fingers brushing the small vial of dust tucked safely in the pocket of your jacket. The pulse in your chest quickens, and you force yourself to step closer.&lt;br /&gt; &lt;br /&gt; “I know why you’re in pain,” you say, the words shaking slightly but firm. “I know what you lost—your wife, your son. I won’t face you in the torment of your grief but in the truth of it.”&lt;br /&gt; &lt;br /&gt; Still, he does not move. The snowman at his side seems to leer at you with a fixed, hollow expression, its eyes dark holes that echo the cold dread creeping into your veins. The wind howls louder, rattling the branches like the rattling of old bones. The air thickens with frost, pressing against you until it feels like a weight on your chest.&lt;br /&gt; &lt;br /&gt; You stop just short of him, feet planted in the snow. “Face me!” The demand comes out with more desperation than you intend, and the stillness of his response gnaws at your resolve.&lt;br /&gt; &lt;br /&gt; Realization settles in—you need something else. Something to break through this stalemate, a shield against his icy silence. You cast your eyes around the desolate lot, searching for anything, but the emptiness is suffocating. Your fingers tighten around the vial of dust, your last hope wrapped in fragile glass.&lt;br /&gt; &lt;br /&gt; Suddenly, you take a step back, turning away as if in defeat, your heart pounding. The silence stretches thin until, just as you move to leave, his voice reaches you—a cold, hollow whisper that cuts through the wind.&lt;br /&gt; &lt;br /&gt; “Face me, child. Face me…”&lt;br /&gt; &lt;br /&gt; A shiver runs down your spine, not from the cold but from the sound of his voice, a chilling mix of command and plea. You turn back, meeting the gaze of The Frozen King. This is it, you think. The moment to either confront the darkness or be swallowed by it.</t>
+  </si>
+  <si>
+    <t>You went looking for the shield and found it on a beast in the shadows of the snowstorm that seemed to be sweeping across the land.&lt;br /&gt; &lt;br /&gt; Returning to the lot, you see him, The Frozen King, still standing where you left him. You approach him and feel the wind picking up, the ice chips in the wind cutting your skin. You raise the shield, and while you no longer feel the ice chips, you do feel the chill of the wind. You hear the howl of the wind, his wife’s voice, her sadness.&lt;br /&gt; &lt;br /&gt; You get closer to him and see him raise his sword toward you.&lt;br /&gt; &lt;br /&gt; “Face me, child.”&lt;br /&gt; &lt;br /&gt; You take the vial and throw it. You throw it at the snowman, not knowing if this is an aspect of him, but something inside you screams to throw it at the snowman. The wind and the ice shards, now swirling fiercely, strike the vial. It shatters, and he starts to laugh.&lt;br /&gt; &lt;br /&gt; The dust manages to hit the snowman, and it explodes, throwing you both back.&lt;br /&gt; &lt;br /&gt; He screams in rage, in pain, in terror. You hold the shield up, and the avalanche of snow, ice, and sorrow is blocked by it. You hold your ground as best as you can while summoning your magic, calling upon everything you have. In a moment, you both unleash your magic, which radiates across the lot in an immense explosion.&lt;br /&gt; &lt;br /&gt; There is a blinding white light, a shrieking sound, a scream on the wind, and then darkness.&lt;br /&gt; &lt;br /&gt; In the darkness, you see a man step toward you, a man dressed in a black suit. His hair is combed back, his face slender and aged, that of a father.&lt;br /&gt; &lt;br /&gt; “You found the truth of my pain, child. You found a way to reunite me with my child, my wife.” After a moment, he seems to slip backward, and a woman with beautiful golden hair stands next to him. A boy no older than fifteen stands between them, smiling, bringing a warmth to your heart.&lt;br /&gt; &lt;br /&gt; “We are the sliver of hope he holds on to,” he states as he and his wife look at the smiling boy, whose face becomes bloodied, twisted, and dark.&lt;br /&gt; &lt;br /&gt; The woman looks at you and whispers on the cold wind: “Bring him back to us. Let us rest.”&lt;br /&gt; &lt;br /&gt; With that, you awaken in the cold of the night. Lying on the ground, there is nothing but silence in the air.</t>
+  </si>
+  <si>
+    <t>Sliver of humanity</t>
+  </si>
+  <si>
+    <t>You lay on the ground, waiting for any sign of movement. Maybe The Frozen King is not dead. Maybe he waits for your next move. You glance over and see the shield, shattered. You know its magic is lost, dissipated in the cold chill of the night.&lt;br /&gt; &lt;br /&gt; “Are you alive?”&lt;br /&gt; &lt;br /&gt; You look up and see a man standing there. You recognize him. The Wandering Merchant.&lt;br /&gt; &lt;br /&gt; Slowly, you rise to greet this old man—another figure like The Poet who can change his age, his form at will. Sometimes he appears old, sometimes young, but this time, he stands as a middle-aged man, holding a staff and a backpack filled with what you assume are his goods for sale.&lt;br /&gt; &lt;br /&gt; “I thought maybe you had died, child. Good thing you haven’t.”&lt;br /&gt; &lt;br /&gt; You ask him how he got there, what he is doing in this place.&lt;br /&gt; &lt;br /&gt; “I am everywhere. I have goods to sell, child. I came because I felt a chill, a chill that crept into my bones. I knew at once I must come and see if it was true. Once I arrived, I knew it to be true: The Enchanted Snowman is no more. The Frozen King is free.”&lt;br /&gt; &lt;br /&gt; You look around and see the remnants of the exploded snowman. You continue searching for The Frozen King, but he is nowhere to be seen. No trace of his body, nothing.&lt;br /&gt; &lt;br /&gt; You turn back to The Wandering Merchant and ask him what you should do now.&lt;br /&gt; &lt;br /&gt; “You find the sliver of hope, child. As the cats and The Father have said, just as The Mother asked. You find the sliver of hope.”</t>
+  </si>
+  <si>
+    <t>You stand there, staring at him. How are you supposed to do that? What started as an attempt to uncover who The Creator is led you on a journey across various planes and now, through snow, wind, and rage, to this place—a place where people are frozen in their fear of letting go. How are you supposed to find a sliver of hope to save, stop, or do whatever needs to be done with The Creator?&lt;br /&gt; &lt;br /&gt; You stand at a fork in the road with no idea which path to take. You seek The Wandering Merchant’s help, his guidance, and ask him what to do next.&lt;br /&gt; &lt;br /&gt; “Seek out the Frozen Soul.”&lt;br /&gt; &lt;br /&gt; A what?&lt;br /&gt; &lt;br /&gt; “The Frozen Soul,” he repeats.&lt;br /&gt; &lt;br /&gt; What or who is that?&lt;br /&gt; &lt;br /&gt; “It is a soul fragment of The Child. Seek it out, ask your questions, and find a way to fulfill the task you’ve been given. A mother’s request is not something to be ignored, child.”&lt;br /&gt; &lt;br /&gt; With that, he vanishes, as the wind blows past and the chill of the night pierces your mind and soul.</t>
   </si>
 </sst>
 </file>
@@ -3471,7 +3540,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AG236"/>
+  <dimension ref="A1:AG241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -13679,6 +13748,253 @@
         <v>5</v>
       </c>
     </row>
+    <row r="237" spans="1:33">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C237" t="s">
+        <v>645</v>
+      </c>
+      <c r="D237" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E237" t="s">
+        <v>731</v>
+      </c>
+      <c r="H237" t="s">
+        <v>1041</v>
+      </c>
+      <c r="M237" t="s">
+        <v>1042</v>
+      </c>
+      <c r="N237">
+        <v>100000</v>
+      </c>
+      <c r="O237">
+        <v>10000</v>
+      </c>
+      <c r="P237">
+        <v>1000000</v>
+      </c>
+      <c r="Q237">
+        <v>500</v>
+      </c>
+      <c r="T237">
+        <v>1</v>
+      </c>
+      <c r="AA237" t="s">
+        <v>1043</v>
+      </c>
+      <c r="AB237" t="s">
+        <v>1044</v>
+      </c>
+      <c r="AC237" t="s">
+        <v>1040</v>
+      </c>
+      <c r="AD237" t="s">
+        <v>731</v>
+      </c>
+      <c r="AE237">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:33">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C238" t="s">
+        <v>592</v>
+      </c>
+      <c r="D238" t="s">
+        <v>1040</v>
+      </c>
+      <c r="H238" t="s">
+        <v>1046</v>
+      </c>
+      <c r="M238" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N238">
+        <v>100000</v>
+      </c>
+      <c r="O238">
+        <v>10000</v>
+      </c>
+      <c r="P238">
+        <v>1000000</v>
+      </c>
+      <c r="Q238">
+        <v>500</v>
+      </c>
+      <c r="U238" t="s">
+        <v>1039</v>
+      </c>
+      <c r="V238" t="s">
+        <v>1042</v>
+      </c>
+      <c r="AA238" t="s">
+        <v>1048</v>
+      </c>
+      <c r="AB238" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AC238" t="s">
+        <v>1040</v>
+      </c>
+      <c r="AE238">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:33">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C239" t="s">
+        <v>645</v>
+      </c>
+      <c r="D239" t="s">
+        <v>1040</v>
+      </c>
+      <c r="H239" t="s">
+        <v>1047</v>
+      </c>
+      <c r="M239" t="s">
+        <v>1051</v>
+      </c>
+      <c r="N239">
+        <v>100000</v>
+      </c>
+      <c r="O239">
+        <v>1000</v>
+      </c>
+      <c r="P239">
+        <v>1000000</v>
+      </c>
+      <c r="Q239">
+        <v>500</v>
+      </c>
+      <c r="U239" t="s">
+        <v>1045</v>
+      </c>
+      <c r="V239" t="s">
+        <v>1052</v>
+      </c>
+      <c r="AA239" t="s">
+        <v>1053</v>
+      </c>
+      <c r="AB239" t="s">
+        <v>1054</v>
+      </c>
+      <c r="AC239" t="s">
+        <v>1040</v>
+      </c>
+      <c r="AE239">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:33">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C240" t="s">
+        <v>723</v>
+      </c>
+      <c r="D240" t="s">
+        <v>1040</v>
+      </c>
+      <c r="H240" t="s">
+        <v>1051</v>
+      </c>
+      <c r="N240">
+        <v>100000</v>
+      </c>
+      <c r="O240">
+        <v>100000</v>
+      </c>
+      <c r="P240">
+        <v>1000000000</v>
+      </c>
+      <c r="Q240">
+        <v>1000</v>
+      </c>
+      <c r="U240" t="s">
+        <v>1050</v>
+      </c>
+      <c r="V240" t="s">
+        <v>1056</v>
+      </c>
+      <c r="AA240" t="s">
+        <v>1057</v>
+      </c>
+      <c r="AB240" t="s">
+        <v>1058</v>
+      </c>
+      <c r="AC240" t="s">
+        <v>1040</v>
+      </c>
+      <c r="AE240">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:33">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C241" t="s">
+        <v>103</v>
+      </c>
+      <c r="D241" t="s">
+        <v>1040</v>
+      </c>
+      <c r="N241">
+        <v>250000</v>
+      </c>
+      <c r="O241">
+        <v>100000</v>
+      </c>
+      <c r="P241">
+        <v>2000000000</v>
+      </c>
+      <c r="Q241">
+        <v>2000</v>
+      </c>
+      <c r="U241" t="s">
+        <v>1055</v>
+      </c>
+      <c r="AA241" t="s">
+        <v>1060</v>
+      </c>
+      <c r="AB241" t="s">
+        <v>1061</v>
+      </c>
+      <c r="AC241" t="s">
+        <v>1040</v>
+      </c>
+      <c r="AE241">
+        <v>3</v>
+      </c>
+      <c r="AF241" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG241">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the final of the bishop quests.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Quests/quests.xlsx
+++ b/resources/data-imports/Quests/quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1240">
   <si>
     <t>id</t>
   </si>
@@ -3647,15 +3647,45 @@
     <t>You return with everything you need. The Construct stands before you and asks if you have the incantation. You hand it over and confirm that you have gathered the rest of the items.&lt;br /&gt; &lt;br /&gt; "We can start the ritual now, child. We will need to draw him out—draw him here, to this cemetery."&lt;br /&gt; &lt;br /&gt; You ask about the blood he promised.&lt;br /&gt; &lt;br /&gt; "I have it, child. But it is the last thing we add. We must do this in a very particular order. Are you ready?"&lt;br /&gt; &lt;br /&gt; You nod. Judgment Day has come for the Bishop.</t>
   </si>
   <si>
+    <t>The censer and the shock</t>
+  </si>
+  <si>
+    <t>Holy Bejeweled Censer</t>
+  </si>
+  <si>
+    <t>Both you and the Construct are ready to begin the ritual—to open the gates, to banish the Bishop. You’ve both agreed that the ritual alone will be enough to draw him out, but you warned the Construct that the visions might return. You may find it difficult to break free from them. You could become entangled, trapped, unable to return to reality.&lt;br /&gt; &lt;br /&gt; "I understand your fears, child. But I can reach you wherever you might be, no matter what he tries to throw at us. I only ask that you have faith in me, child. Faith in my ability to guide us through this—one last time."&lt;br /&gt; &lt;br /&gt; Ironic, coming from what used to be a Faithless Child. Alas, you agree and hand over the censer.&lt;br /&gt; &lt;br /&gt; "We must now purify the area—create a place where we can begin. I’ll fetch a bowl. Wait here, and I’ll be back."</t>
+  </si>
+  <si>
+    <t>As the incense burns, you wait for the Emerald Soul to return. The silence of the graveyard washes over you—but within moments, it hits. The visions.&lt;br /&gt; &lt;br /&gt; You find yourself lost in darkness, only to awaken in the room—the same room as the man in the white coat, the one you now know as the Corrupted Bishop.&lt;br /&gt; &lt;br /&gt; He sits at a table with a woman and a man—a mother and a father. You recognize them. The Child’s parents. Both were supposed to have died in a car accident one wintry night, not long after the Child took his own life.&lt;br /&gt; &lt;br /&gt; They ended up in a frozen wasteland, corrupted by their own pain and grief, seeking only to be reunited.&lt;br /&gt; &lt;br /&gt; They sit together at a table. You try to call out, but once again—you are merely a spectator.&lt;br /&gt; &lt;br /&gt; "It is obvious to me that your son has experienced great trauma in attempting to take his own life. Instead of facing that reality, he hides in his mind, in what he writes—a twisted fantasy story about some kind of Poet and the like, a war between a Federation, the Church, and a rebellious group. It is my understanding that he is using this world to escape reality. The only way to make him face the truth is to shock him back into it. With that said, I suggest electroshock therapy."&lt;br /&gt; &lt;br /&gt; The mother gasps. "Is it safe? Will it help?"&lt;br /&gt; &lt;br /&gt; The father tries to comfort her, placing his hand on hers. She looks at him, worry clouding her eyes—worry for her child.&lt;br /&gt; &lt;br /&gt; "I assure you, it’s quite safe."&lt;br /&gt; &lt;br /&gt; The vision shifts. The Child lies on a bed. Strange devices are strapped to his head. He is no longer faceless—you know his face. You know him as the Creator. Wires run from the devices to a machine nearby. The doctor pushes a button.&lt;br /&gt; &lt;br /&gt; Your vision blurs.&lt;br /&gt; &lt;br /&gt; The darkness shakes.&lt;br /&gt; &lt;br /&gt; You awaken back in the cemetery—but the ground trembles beneath you. The world itself seems to lurch. Tombstones topple. The very earth shifts.&lt;br /&gt; &lt;br /&gt; The Construct appears, carrying the bowl. It floats toward the unsteady ground.&lt;br /&gt; &lt;br /&gt; "What is happening, child?" he calls out.&lt;br /&gt; &lt;br /&gt; Something about the shock—the Bishop—he’s shocking the Child…&lt;br /&gt; &lt;br /&gt; "What?!" the Construct exclaims in confusion.&lt;br /&gt; &lt;br /&gt; You tell him to continue with the ritual.</t>
+  </si>
+  <si>
+    <t>Maladaptive Daydreaming</t>
+  </si>
+  <si>
+    <t>Chains of The River Man</t>
+  </si>
+  <si>
+    <t>The ground continues to shake. The incense burns. The Emerald Soul instructs you to place the chains into the bowl. He will give you the blood needed to pour over them—after you read the ritual.&lt;br /&gt; &lt;br /&gt; You place the chains in the bowl, and the ground ruptures. It cracks open. A scream erupts from the sky—a wailing, gut-wrenching cry. The world fades in and out of darkness.&lt;br /&gt; &lt;br /&gt; You shout to the Construct to start chanting.&lt;br /&gt; &lt;br /&gt; That’s when he appears.&lt;br /&gt; &lt;br /&gt; The Corrupted Bishop.&lt;br /&gt; &lt;br /&gt; A man dressed in red robes, wearing a tall mitre upon his head.&lt;br /&gt; &lt;br /&gt; "Child! What do you and your little godless heathen friend think you are doing?"&lt;br /&gt; &lt;br /&gt; You look at the Emerald Soul. You hear his chanting falter.&lt;br /&gt; &lt;br /&gt; You scream at him to continue.&lt;br /&gt; &lt;br /&gt; The Bishop reaches out—and you are hit with immense pain. The visions return.</t>
+  </si>
+  <si>
+    <t>A mother sits at the bedside of her sleeping child. She weeps for her baby.&lt;br /&gt; &lt;br /&gt; A father stands in the hallway. He cries tears of guilt—for his failure to guide, to protect, to love his child.&lt;br /&gt; &lt;br /&gt; The man in the white coat sits in his office.&lt;br /&gt; &lt;br /&gt; And you sit across from him.&lt;br /&gt; &lt;br /&gt; You both face each other in silence.&lt;br /&gt; &lt;br /&gt; "What is it you think you’ll accomplish with your little magical spell?" he asks. His voice is calm. He holds a notepad and pen, waiting for your response.&lt;br /&gt; &lt;br /&gt; You tell him you now understand—it’s all connected. You tell him that when you saw him shock the Child, the world—the one you’re from—began to shake, began to…&lt;br /&gt; &lt;br /&gt; Your words trail off.&lt;br /&gt; &lt;br /&gt; "The world you’re from? The fantasy? The delusion? The place he escapes to in order to avoid reality? To escape the pain and suffering he still causes through his inability to accept what he’s done—the trauma he’s inflicted on his own parents?"&lt;br /&gt; &lt;br /&gt; He writes something down before continuing.&lt;br /&gt; &lt;br /&gt; "Why are you so invested in all of this? What do you hope to gain? Do you really think you’ll banish me? Is that what you’re doing? Sitting in your room, muttering to yourself, spinning stories about the big, bad Corrupted Bishop.&lt;br /&gt; &lt;br /&gt; "Am I him? Am I the Bishop?&lt;br /&gt; &lt;br /&gt; "I’m just trying to help you. Help you get better. But you don’t want to help yourself."&lt;br /&gt; &lt;br /&gt; You tell him none of this is real. It’s all part of his corrupted alchemy—his twisted old-world science. His failed experiments on children. The torment he’s put them through—emotionally, mentally, physically, and…&lt;br /&gt; &lt;br /&gt; You can’t even say it. You know the words. But you won’t let yourself go there.&lt;br /&gt; &lt;br /&gt; "You’ve befriended the Child over these months. Fed into his delusions. You were making progress. But now you’re back to weaving fanciful tales. Do you even know why you’re here, in this hospital? Do you know what mental affliction you suffer from?"&lt;br /&gt; &lt;br /&gt; He pauses. Jots something down. Looks at you, waiting.&lt;br /&gt; &lt;br /&gt; You fight as hard as you can to break free of his spell—his twisted illusion.&lt;br /&gt; &lt;br /&gt; "Maladaptive Daydreaming. Do you know what that is?&lt;br /&gt; &lt;br /&gt; "It’s when you lose yourself in complex daydreams. You were molested as a child. Beaten. Left to fend for yourself. And you cope by living in these complex fantasies—they’re nothing more than a coping mechanism. I’m here to help you break free, to face your trauma, and begin healing."&lt;br /&gt; &lt;br /&gt; Suddenly, the room begins to shake. His face begins to warp—shifting back and forth between the calm doctor and the Bishop in red robes.&lt;br /&gt; &lt;br /&gt; "Can you not see what is real and what isn’t, child?"&lt;br /&gt; &lt;br /&gt; You force yourself to look beyond the illusion—to see the Bishop standing in the graveyard. You hear the chanting of the Emerald Soul. It continues.&lt;br /&gt; &lt;br /&gt; You reach through the vision—toward your reality. Toward what you know is true.&lt;br /&gt; &lt;br /&gt; You tell the Bishop, if he wants to look upon the face of God… then you shall let him.&lt;br /&gt; &lt;br /&gt; You conjure the magic of your gear—your weapons, your armor, your soul—and you hurl it all at the Bishop. He stumbles back.&lt;br /&gt; &lt;br /&gt; The vision breaks.&lt;br /&gt; &lt;br /&gt; You scream at the Construct for the blood.</t>
+  </si>
+  <si>
+    <t>The end of the delusions</t>
+  </si>
+  <si>
+    <t>With the Bishop knocked back, the Emerald Construct floats the vial of blood toward you. You grab it and race to the bowl. The Bishop rises and screams.&lt;br /&gt; You throw the vial—&lt;br /&gt; &lt;br /&gt; And suddenly, you’re back in the hospital. Back in the vision.&lt;br /&gt; &lt;br /&gt; This time, you’re strapped to a bed. The doctor stands nearby.&lt;br /&gt; &lt;br /&gt; "You are being restrained for your own safety. You tried to attack me in the office—do you remember that?"&lt;br /&gt; &lt;br /&gt; You scream at him. You shout that he is the Bishop, that he cannot be allowed to look upon the face of God.&lt;br /&gt; &lt;br /&gt; "When you calm down, we can talk more about these delusions."&lt;br /&gt; &lt;br /&gt; He turns and leaves the room. You’re alone. Trapped. Bound to the bed. You struggle, but you can’t break free.&lt;br /&gt; &lt;br /&gt; You look around. It’s a plain, nondescript room with four walls, a window, a small nightstand, and the bed you’re confined to.&lt;br /&gt; &lt;br /&gt; For the first time in all your adventures—across all the planes you’ve traveled—you feel utterly helpless.&lt;br /&gt; &lt;br /&gt; A moment later, the door creaks open, and an older man walks in. You recognize his face, but he looks different now—dressed like a grandfather.&lt;br /&gt; &lt;br /&gt; "Hello, my child," he says as he approaches and sits at the edge of the bed.&lt;br /&gt; &lt;br /&gt; You ask him who he is, what he wants, why he’s here. But you can’t shake the feeling that you know him.&lt;br /&gt; &lt;br /&gt; "You need to wake up," he says, his voice soft and caring.&lt;br /&gt; &lt;br /&gt; "You need to wake up and finish what you started. It’s happening."&lt;br /&gt; &lt;br /&gt; You tell him you don’t understand. But suddenly, your eyes grow heavy. Exhaustion takes over.&lt;br /&gt; &lt;br /&gt; You drift into darkness.</t>
+  </si>
+  <si>
+    <t>A bright light shines in the sky. It radiates across the land.&lt;br /&gt; &lt;br /&gt; As your eyes open, it looks like a beam from the heavens themselves. Then you realize what’s happening.&lt;br /&gt; &lt;br /&gt; The gates are opening.&lt;br /&gt; &lt;br /&gt; The Emerald Soul is slowly fading.&lt;br /&gt; &lt;br /&gt; "Thank you, child. You have set me free," it says.&lt;br /&gt; &lt;br /&gt; And then, it vanishes.&lt;br /&gt; &lt;br /&gt; The light grows brighter.&lt;br /&gt; &lt;br /&gt; The Bishop stands. He walks toward the beam of light. You rise as well, pulling a weapon from your side. You ready it.&lt;br /&gt; &lt;br /&gt; He laughs and continues walking into the beam.&lt;br /&gt; &lt;br /&gt; You feel the heat, the love, the radiance pouring from it.&lt;br /&gt; &lt;br /&gt; He stretches his arms wide, lifts his head high.&lt;br /&gt; &lt;br /&gt; "I am ready, Lord! I am ready to face—"&lt;br /&gt; &lt;br /&gt; He stops. Looks down.&lt;br /&gt; &lt;br /&gt; Your weapon juts from his belly.&lt;br /&gt; &lt;br /&gt; You rip it back. Blood pours from his mouth.&lt;br /&gt; &lt;br /&gt; The beam lifts him up.&lt;br /&gt; &lt;br /&gt; And then, in a moment—&lt;br /&gt; &lt;br /&gt; Silence.&lt;br /&gt; &lt;br /&gt; The light is gone.&lt;br /&gt; &lt;br /&gt; The Bishop is gone.&lt;br /&gt; &lt;br /&gt; Did you do it?&lt;br /&gt; &lt;br /&gt; Is it over?&lt;br /&gt; &lt;br /&gt; Are you home?&lt;br /&gt; &lt;br /&gt; Is this reality?&lt;br /&gt; &lt;br /&gt; You collapse.&lt;br /&gt; &lt;br /&gt; And begin to weep.</t>
+  </si>
+  <si>
     <t>Chains of the past</t>
   </si>
   <si>
     <t>Soldierofthegates</t>
   </si>
   <si>
-    <t>Chains of The River Man</t>
-  </si>
-  <si>
     <t>You arrive back in Purgatory, at the Cellar—but alas, it’s empty. Even the chains are gone. There’s no one here.&lt;br /&gt; &lt;br /&gt; You leave the Cellar and look around, only to see a man standing not far from the entrance. You cautiously approach him. He greets you.&lt;br /&gt; &lt;br /&gt; "Hello, child."&lt;br /&gt; &lt;br /&gt; He looks slightly older than you—fit, dressed in a tunic and leather pants. He carries a sword and a lantern.&lt;br /&gt; &lt;br /&gt; You’ve never seen him before and ask who he is.&lt;br /&gt; &lt;br /&gt; "I am a Soldier of the Gates. I seek the man who was in this Cellar. Do you know anything about him?"&lt;br /&gt; &lt;br /&gt; You begin to explain the ritual, the Key Maker, and how you asked the River Man about it—but you’re cut off by an angry outburst.&lt;br /&gt; &lt;br /&gt; "You did what?! Are you stupid? Do you not know what you’ve done?!"&lt;br /&gt; &lt;br /&gt; You try to explain what the Construct told you and how you planned to fix the mess after dealing with the Bishop, but the Soldier of the Gates isn’t having it.&lt;br /&gt; &lt;br /&gt; "Enough, child! You have done irrevocable harm here today with your idiocy! You stuck your nose where it doesn’t belong and unleashed a madman—an escapee from Heaven itself. Do you know what this means?!"&lt;br /&gt; &lt;br /&gt; You sarcastically state that you’re a thousand steps away from discovering the truth of the Child—but also one step closer.&lt;br /&gt; &lt;br /&gt; "YOU BAFFLING IDIOT!" he yells.&lt;br /&gt; &lt;br /&gt; He starts to storm off. You call after him, asking if he knows where the River Man’s chains are because you need them. He stops and turns.&lt;br /&gt; &lt;br /&gt; "What the hell would you need those for?"&lt;br /&gt; &lt;br /&gt; You begin to tell him how you plan to stop the Corrupted Bishop.</t>
   </si>
   <si>
@@ -3669,9 +3699,6 @@
   </si>
   <si>
     <t>Thieves Tool Kit</t>
-  </si>
-  <si>
-    <t>Holy Bejeweled Censer</t>
   </si>
   <si>
     <t>Mothers Sleep</t>
@@ -4047,7 +4074,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AG278"/>
+  <dimension ref="A1:AG281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -16079,43 +16106,40 @@
     </row>
     <row r="275" spans="1:33">
       <c r="A275">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B275" t="s">
         <v>1210</v>
       </c>
       <c r="C275" t="s">
-        <v>1211</v>
+        <v>1028</v>
       </c>
       <c r="D275" t="s">
         <v>1201</v>
       </c>
-      <c r="G275">
-        <v>20</v>
-      </c>
-      <c r="M275" t="s">
+      <c r="H275" t="s">
+        <v>1211</v>
+      </c>
+      <c r="N275">
+        <v>200000</v>
+      </c>
+      <c r="O275">
+        <v>200000</v>
+      </c>
+      <c r="P275">
+        <v>2000000000</v>
+      </c>
+      <c r="Q275">
+        <v>2000</v>
+      </c>
+      <c r="U275" t="s">
+        <v>1205</v>
+      </c>
+      <c r="AA275" t="s">
         <v>1212</v>
       </c>
-      <c r="N275">
-        <v>100000</v>
-      </c>
-      <c r="O275">
-        <v>100000</v>
-      </c>
-      <c r="P275">
-        <v>1000000000</v>
-      </c>
-      <c r="Q275">
-        <v>1250</v>
-      </c>
-      <c r="U275" t="s">
-        <v>1200</v>
-      </c>
-      <c r="AA275" t="s">
+      <c r="AB275" t="s">
         <v>1213</v>
-      </c>
-      <c r="AB275" t="s">
-        <v>1214</v>
       </c>
       <c r="AC275" t="s">
         <v>1201</v>
@@ -16124,54 +16148,48 @@
         <v>7</v>
       </c>
       <c r="AF275" t="s">
-        <v>1211</v>
+        <v>1028</v>
       </c>
       <c r="AG275">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="276" spans="1:33">
       <c r="A276">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B276" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="C276" t="s">
-        <v>1216</v>
+        <v>1028</v>
       </c>
       <c r="D276" t="s">
         <v>1201</v>
       </c>
       <c r="H276" t="s">
-        <v>1217</v>
-      </c>
-      <c r="M276" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="N276">
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="O276">
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="P276">
-        <v>1000000000</v>
+        <v>2000000000</v>
       </c>
       <c r="Q276">
-        <v>1350</v>
+        <v>2500</v>
       </c>
       <c r="U276" t="s">
         <v>1210</v>
       </c>
-      <c r="V276" t="s">
-        <v>1219</v>
-      </c>
       <c r="AA276" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="AB276" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="AC276" t="s">
         <v>1201</v>
@@ -16179,52 +16197,52 @@
       <c r="AE276">
         <v>7</v>
       </c>
-      <c r="AF276" t="s">
-        <v>1216</v>
-      </c>
-      <c r="AG276">
-        <v>3</v>
-      </c>
     </row>
     <row r="277" spans="1:33">
       <c r="A277">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B277" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="C277" t="s">
-        <v>842</v>
+        <v>1028</v>
       </c>
       <c r="D277" t="s">
         <v>1201</v>
       </c>
-      <c r="H277" t="s">
-        <v>1223</v>
-      </c>
-      <c r="M277" t="s">
-        <v>1224</v>
+      <c r="I277">
+        <v>1000</v>
+      </c>
+      <c r="J277">
+        <v>1000</v>
+      </c>
+      <c r="K277">
+        <v>2000000</v>
+      </c>
+      <c r="L277">
+        <v>1000</v>
       </c>
       <c r="N277">
-        <v>150000</v>
+        <v>400000</v>
       </c>
       <c r="O277">
-        <v>150000</v>
+        <v>400000</v>
       </c>
       <c r="P277">
-        <v>1500000000</v>
+        <v>4000000000</v>
       </c>
       <c r="Q277">
-        <v>1500</v>
+        <v>5000</v>
       </c>
       <c r="U277" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="AA277" t="s">
-        <v>1225</v>
+        <v>1219</v>
       </c>
       <c r="AB277" t="s">
-        <v>1226</v>
+        <v>1220</v>
       </c>
       <c r="AC277" t="s">
         <v>1201</v>
@@ -16235,51 +16253,207 @@
     </row>
     <row r="278" spans="1:33">
       <c r="A278">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B278" t="s">
-        <v>1227</v>
+        <v>1221</v>
       </c>
       <c r="C278" t="s">
-        <v>38</v>
+        <v>1222</v>
       </c>
       <c r="D278" t="s">
         <v>1201</v>
       </c>
-      <c r="H278" t="s">
+      <c r="G278">
+        <v>20</v>
+      </c>
+      <c r="M278" t="s">
+        <v>1215</v>
+      </c>
+      <c r="N278">
+        <v>100000</v>
+      </c>
+      <c r="O278">
+        <v>100000</v>
+      </c>
+      <c r="P278">
+        <v>1000000000</v>
+      </c>
+      <c r="Q278">
+        <v>1250</v>
+      </c>
+      <c r="U278" t="s">
+        <v>1200</v>
+      </c>
+      <c r="AA278" t="s">
+        <v>1223</v>
+      </c>
+      <c r="AB278" t="s">
         <v>1224</v>
-      </c>
-      <c r="M278" t="s">
-        <v>1207</v>
-      </c>
-      <c r="N278">
-        <v>150000</v>
-      </c>
-      <c r="O278">
-        <v>150000</v>
-      </c>
-      <c r="P278">
-        <v>1500000000</v>
-      </c>
-      <c r="Q278">
-        <v>1500</v>
-      </c>
-      <c r="U278" t="s">
-        <v>1222</v>
-      </c>
-      <c r="V278" t="s">
-        <v>1228</v>
-      </c>
-      <c r="AA278" t="s">
-        <v>1229</v>
-      </c>
-      <c r="AB278" t="s">
-        <v>1230</v>
       </c>
       <c r="AC278" t="s">
         <v>1201</v>
       </c>
       <c r="AE278">
+        <v>7</v>
+      </c>
+      <c r="AF278" t="s">
+        <v>1222</v>
+      </c>
+      <c r="AG278">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:33">
+      <c r="A279">
+        <v>275</v>
+      </c>
+      <c r="B279" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C279" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D279" t="s">
+        <v>1201</v>
+      </c>
+      <c r="H279" t="s">
+        <v>1227</v>
+      </c>
+      <c r="M279" t="s">
+        <v>1211</v>
+      </c>
+      <c r="N279">
+        <v>100000</v>
+      </c>
+      <c r="O279">
+        <v>100000</v>
+      </c>
+      <c r="P279">
+        <v>1000000000</v>
+      </c>
+      <c r="Q279">
+        <v>1350</v>
+      </c>
+      <c r="U279" t="s">
+        <v>1221</v>
+      </c>
+      <c r="V279" t="s">
+        <v>1228</v>
+      </c>
+      <c r="AA279" t="s">
+        <v>1229</v>
+      </c>
+      <c r="AB279" t="s">
+        <v>1230</v>
+      </c>
+      <c r="AC279" t="s">
+        <v>1201</v>
+      </c>
+      <c r="AE279">
+        <v>7</v>
+      </c>
+      <c r="AF279" t="s">
+        <v>1226</v>
+      </c>
+      <c r="AG279">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:33">
+      <c r="A280">
+        <v>276</v>
+      </c>
+      <c r="B280" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C280" t="s">
+        <v>842</v>
+      </c>
+      <c r="D280" t="s">
+        <v>1201</v>
+      </c>
+      <c r="H280" t="s">
+        <v>1232</v>
+      </c>
+      <c r="M280" t="s">
+        <v>1233</v>
+      </c>
+      <c r="N280">
+        <v>150000</v>
+      </c>
+      <c r="O280">
+        <v>150000</v>
+      </c>
+      <c r="P280">
+        <v>1500000000</v>
+      </c>
+      <c r="Q280">
+        <v>1500</v>
+      </c>
+      <c r="U280" t="s">
+        <v>1225</v>
+      </c>
+      <c r="AA280" t="s">
+        <v>1234</v>
+      </c>
+      <c r="AB280" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AC280" t="s">
+        <v>1201</v>
+      </c>
+      <c r="AE280">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="281" spans="1:33">
+      <c r="A281">
+        <v>277</v>
+      </c>
+      <c r="B281" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C281" t="s">
+        <v>38</v>
+      </c>
+      <c r="D281" t="s">
+        <v>1201</v>
+      </c>
+      <c r="H281" t="s">
+        <v>1233</v>
+      </c>
+      <c r="M281" t="s">
+        <v>1207</v>
+      </c>
+      <c r="N281">
+        <v>150000</v>
+      </c>
+      <c r="O281">
+        <v>150000</v>
+      </c>
+      <c r="P281">
+        <v>1500000000</v>
+      </c>
+      <c r="Q281">
+        <v>1500</v>
+      </c>
+      <c r="U281" t="s">
+        <v>1231</v>
+      </c>
+      <c r="V281" t="s">
+        <v>1237</v>
+      </c>
+      <c r="AA281" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AB281" t="s">
+        <v>1239</v>
+      </c>
+      <c r="AC281" t="s">
+        <v>1201</v>
+      </c>
+      <c r="AE281">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Put in the last quest with the new item.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Quests/quests.xlsx
+++ b/resources/data-imports/Quests/quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1243">
   <si>
     <t>id</t>
   </si>
@@ -3735,6 +3735,15 @@
   </si>
   <si>
     <t>You never thought to ask what the book was for—or what was written inside. Now you stand aboard a wrecked ship, staring down at it. You flip through the pages, hoping to glean something of value.&lt;br /&gt; &lt;br /&gt; That’s when you hear her voice.&lt;br /&gt; &lt;br /&gt; "Oh, child. You shouldn’t be reading other people’s personal entries. It’s not nice to snoop."&lt;br /&gt; &lt;br /&gt; Before you can respond, the pages go blank—and you find yourself standing before her once again.&lt;br /&gt; &lt;br /&gt; She snatches the book from your hands and tosses it into the fire. You ask her why, but she only shrugs and turns away. She walks over to a rotting dresser, barely holding itself together, full of holes and decay. She opens the second drawer from the top and pulls out a dagger—a bone-white dagger.&lt;br /&gt; &lt;br /&gt; "A deal is a deal," she says, handing you the weapon.&lt;br /&gt; &lt;br /&gt; "Off to see the Witch—the wonderful Witch of the labyrinth," she cackles, then vanishes.&lt;br /&gt; &lt;br /&gt; What was in the book? Why did she burn it?&lt;br /&gt; &lt;br /&gt; Questions you’ll have to figure out later. Maybe it wasn’t important to the task at hand... or maybe it was.&lt;br /&gt; &lt;br /&gt; Either way, your path is clear: it’s time to find the Witch, and secure the second-to-last item.</t>
+  </si>
+  <si>
+    <t>What now?</t>
+  </si>
+  <si>
+    <t>It has been two weeks since the confrontation with the Bishop. The visions have stopped.&lt;br /&gt; &lt;br /&gt; You’ve wandered from plane to plane, searching for the Soldier of the Gate. You remember the deal you struck with him—but he is nowhere to be found. Not in Purgatory. Not even at the empty Cellar.&lt;br /&gt; &lt;br /&gt; Eventually, you find yourself in a pub on the surface. You sit alone, drinking stale beer, eating dry bread and old cheese, picking off bits of mold.&lt;br /&gt; &lt;br /&gt; You reflect on everything that has happened—between the Ice Queen, the Frozen King, the Jester, and now the Corrupted Bishop. Every encounter has led you down a road you no longer know how to travel. You're exhausted. Worn out. Tired in every way.&lt;br /&gt; &lt;br /&gt; "Hello, child," comes a voice.&lt;br /&gt; &lt;br /&gt; "I’m glad you woke up."&lt;br /&gt; &lt;br /&gt; You look up and see a man. You recognize him. The Wandering Merchant.&lt;br /&gt; &lt;br /&gt; "I’m glad to see you managed to break the spell and banish the Bishop. The delusions can start to fade now. The pain and suffering can finally come to an end. Even as we speak, the Church collapses. The Federation dissolves."&lt;br /&gt; &lt;br /&gt; You ask him if any of it was real.&lt;br /&gt; &lt;br /&gt; "Real? Define real, child. What even is real?"&lt;br /&gt; &lt;br /&gt; You sit there, wondering that very question—what even is real?&lt;br /&gt; &lt;br /&gt; After a moment, the Wandering Merchant stands. He turns and smiles.&lt;br /&gt; &lt;br /&gt; "I am truly glad you woke up, child."&lt;br /&gt; &lt;br /&gt; You smile back, thank him, and tell him you’re glad you woke up too. But then you ask—&lt;br /&gt; &lt;br /&gt; What now?&lt;br /&gt; &lt;br /&gt; "You keep on going," he says.&lt;br /&gt; &lt;br /&gt; He smiles, turns, and walks away.</t>
+  </si>
+  <si>
+    <t>You walk through the marketplace in the town where you had sat in the pub. You watch the people—their faces, their gestures, their conversations. You wonder to yourself how you’re supposed to keep going. Every adventure leads down a road, but none of those roads seem to have answers.&lt;br /&gt; &lt;br /&gt; You feel a tap on your shoulder.&lt;br /&gt; &lt;br /&gt; You turn.&lt;br /&gt; &lt;br /&gt; A hooded man stands before you.&lt;br /&gt; &lt;br /&gt; "Thank you," he says.&lt;br /&gt; &lt;br /&gt; You ask—for what?&lt;br /&gt; &lt;br /&gt; "You saved me. From him. I owe you a debt."&lt;br /&gt; &lt;br /&gt; You ask who he is. You try to peer beneath the hood—but there's nothing there. Just shadows and darkness.&lt;br /&gt; &lt;br /&gt; And in a moment, he’s gone.&lt;br /&gt; &lt;br /&gt; You’re left alone, surrounded by the crowd. Some people glance at you. Others don’t notice you at all.&lt;br /&gt; &lt;br /&gt; You turn.&lt;br /&gt; &lt;br /&gt; And walk on, down the road.</t>
   </si>
 </sst>
 </file>
@@ -4074,7 +4083,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AG281"/>
+  <dimension ref="A1:AG282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -16457,6 +16466,71 @@
         <v>7</v>
       </c>
     </row>
+    <row r="282" spans="1:33">
+      <c r="A282">
+        <v>281</v>
+      </c>
+      <c r="B282" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C282" t="s">
+        <v>103</v>
+      </c>
+      <c r="D282" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E282" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G282">
+        <v>30</v>
+      </c>
+      <c r="I282">
+        <v>1000000</v>
+      </c>
+      <c r="J282">
+        <v>1000000</v>
+      </c>
+      <c r="K282">
+        <v>10000000000</v>
+      </c>
+      <c r="L282">
+        <v>100000</v>
+      </c>
+      <c r="N282">
+        <v>1000000</v>
+      </c>
+      <c r="O282">
+        <v>1000000</v>
+      </c>
+      <c r="P282">
+        <v>100000000000</v>
+      </c>
+      <c r="Q282">
+        <v>5000</v>
+      </c>
+      <c r="U282" t="s">
+        <v>1200</v>
+      </c>
+      <c r="Y282">
+        <v>7</v>
+      </c>
+      <c r="AA282" t="s">
+        <v>1241</v>
+      </c>
+      <c r="AB282" t="s">
+        <v>1242</v>
+      </c>
+      <c r="AC282" t="s">
+        <v>1201</v>
+      </c>
+      <c r="AD282" t="s">
+        <v>1218</v>
+      </c>
+      <c r="AE282">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
We can now have two raids run at the same time across different maps.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Quests/quests.xlsx
+++ b/resources/data-imports/Quests/quests.xlsx
@@ -18174,9 +18174,6 @@
       <c r="C312" t="s">
         <v>1359</v>
       </c>
-      <c r="D312" t="s">
-        <v>1360</v>
-      </c>
       <c r="I312">
         <v>500</v>
       </c>
@@ -18209,9 +18206,6 @@
       </c>
       <c r="AB312" t="s">
         <v>1366</v>
-      </c>
-      <c r="AC312" t="s">
-        <v>1360</v>
       </c>
       <c r="AF312" t="s">
         <v>1359</v>
@@ -18230,9 +18224,6 @@
       <c r="C313" t="s">
         <v>1359</v>
       </c>
-      <c r="D313" t="s">
-        <v>1360</v>
-      </c>
       <c r="H313" t="s">
         <v>1368</v>
       </c>
@@ -18256,9 +18247,6 @@
       </c>
       <c r="AB313" t="s">
         <v>1370</v>
-      </c>
-      <c r="AC313" t="s">
-        <v>1360</v>
       </c>
       <c r="AF313" t="s">
         <v>1359</v>
@@ -18277,9 +18265,6 @@
       <c r="C314" t="s">
         <v>38</v>
       </c>
-      <c r="D314" t="s">
-        <v>1360</v>
-      </c>
       <c r="I314">
         <v>1000</v>
       </c>
@@ -18309,9 +18294,6 @@
       </c>
       <c r="AB314" t="s">
         <v>1373</v>
-      </c>
-      <c r="AC314" t="s">
-        <v>1360</v>
       </c>
       <c r="AF314" t="s">
         <v>38</v>
@@ -18330,9 +18312,6 @@
       <c r="C315" t="s">
         <v>1359</v>
       </c>
-      <c r="D315" t="s">
-        <v>1360</v>
-      </c>
       <c r="H315" t="s">
         <v>1375</v>
       </c>
@@ -18365,9 +18344,6 @@
       </c>
       <c r="AB315" t="s">
         <v>1377</v>
-      </c>
-      <c r="AC315" t="s">
-        <v>1360</v>
       </c>
       <c r="AF315" t="s">
         <v>1359</v>
@@ -18386,9 +18362,6 @@
       <c r="C316" t="s">
         <v>1359</v>
       </c>
-      <c r="D316" t="s">
-        <v>1360</v>
-      </c>
       <c r="N316">
         <v>2000</v>
       </c>
@@ -18409,9 +18382,6 @@
       </c>
       <c r="AB316" t="s">
         <v>1380</v>
-      </c>
-      <c r="AC316" t="s">
-        <v>1360</v>
       </c>
       <c r="AF316" t="s">
         <v>1359</v>
@@ -18430,9 +18400,6 @@
       <c r="C317" t="s">
         <v>38</v>
       </c>
-      <c r="D317" t="s">
-        <v>1360</v>
-      </c>
       <c r="H317" t="s">
         <v>1382</v>
       </c>
@@ -18459,9 +18426,6 @@
       </c>
       <c r="AB317" t="s">
         <v>1385</v>
-      </c>
-      <c r="AC317" t="s">
-        <v>1360</v>
       </c>
       <c r="AF317" t="s">
         <v>38</v>
@@ -18480,9 +18444,6 @@
       <c r="C318" t="s">
         <v>38</v>
       </c>
-      <c r="D318" t="s">
-        <v>1360</v>
-      </c>
       <c r="H318" t="s">
         <v>1387</v>
       </c>
@@ -18506,9 +18467,6 @@
       </c>
       <c r="AB318" t="s">
         <v>1389</v>
-      </c>
-      <c r="AC318" t="s">
-        <v>1360</v>
       </c>
       <c r="AF318" t="s">
         <v>38</v>
@@ -18527,9 +18485,6 @@
       <c r="C319" t="s">
         <v>38</v>
       </c>
-      <c r="D319" t="s">
-        <v>1360</v>
-      </c>
       <c r="I319">
         <v>20000</v>
       </c>
@@ -18559,9 +18514,6 @@
       </c>
       <c r="AB319" t="s">
         <v>1392</v>
-      </c>
-      <c r="AC319" t="s">
-        <v>1360</v>
       </c>
     </row>
     <row r="320" spans="1:33">
@@ -18574,9 +18526,6 @@
       <c r="C320" t="s">
         <v>1394</v>
       </c>
-      <c r="D320" t="s">
-        <v>1360</v>
-      </c>
       <c r="N320">
         <v>4000</v>
       </c>
@@ -18597,9 +18546,6 @@
       </c>
       <c r="AB320" t="s">
         <v>1396</v>
-      </c>
-      <c r="AC320" t="s">
-        <v>1360</v>
       </c>
       <c r="AF320" t="s">
         <v>1394</v>
@@ -18618,9 +18564,6 @@
       <c r="C321" t="s">
         <v>1394</v>
       </c>
-      <c r="D321" t="s">
-        <v>1360</v>
-      </c>
       <c r="N321">
         <v>5000</v>
       </c>
@@ -18644,9 +18587,6 @@
       </c>
       <c r="AB321" t="s">
         <v>1399</v>
-      </c>
-      <c r="AC321" t="s">
-        <v>1360</v>
       </c>
       <c r="AF321" t="s">
         <v>1394</v>

</xml_diff>